<commit_message>
Monthly update on files
</commit_message>
<xml_diff>
--- a/data/hme/raw/hme_report.xlsx
+++ b/data/hme/raw/hme_report.xlsx
@@ -140,26 +140,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFE35454"/>
+        <bgColor rgb="FFE35454"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB40000"/>
+        <bgColor rgb="FFB40000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00B04C"/>
         <bgColor rgb="FF00B04C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE35454"/>
-        <bgColor rgb="FFE35454"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF540202"/>
         <bgColor rgb="FF540202"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB40000"/>
-        <bgColor rgb="FFB40000"/>
       </patternFill>
     </fill>
   </fills>
@@ -291,10 +291,10 @@
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="82" fontId="7" fillId="4" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="82" fontId="7" fillId="5" borderId="1">
+    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="82" fontId="8" fillId="3" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="82" fontId="8" fillId="3" borderId="1">
+    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="82" fontId="7" fillId="5" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="82" fontId="7" fillId="6" borderId="1">
@@ -327,10 +327,13 @@
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="4" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="5" borderId="1">
+    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="7" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="10" fillId="3" borderId="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="5" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="0" fontId="1" fillId="3" borderId="6">
@@ -339,16 +342,13 @@
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="6" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="8" borderId="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="0" fontId="1" fillId="3" borderId="7">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="0" fontId="1" fillId="0" borderId="8">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="7" borderId="1">
+    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="8" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -374,10 +374,10 @@
       <rgbColor rgb="00FFFFFF"/>
       <rgbColor rgb="00333333"/>
       <rgbColor rgb="00F4D216"/>
+      <rgbColor rgb="00E35454"/>
+      <rgbColor rgb="00B40000"/>
       <rgbColor rgb="0000B04C"/>
-      <rgbColor rgb="00E35454"/>
       <rgbColor rgb="00540202"/>
-      <rgbColor rgb="00B40000"/>
       <rgbColor rgb="00808000"/>
       <rgbColor rgb="00800080"/>
       <rgbColor rgb="00008080"/>
@@ -520,7 +520,7 @@
     <row r="3" ht="18.15" customHeight="1">
       <c s="2" t="inlineStr" r="C3">
         <is>
-          <t xml:space="preserve">Day: 11/12/2025</t>
+          <t xml:space="preserve">Day: 11/30/2025</t>
         </is>
       </c>
     </row>
@@ -616,49 +616,49 @@
       <c s="4" t="str" r="C7"/>
       <c s="5" t="str" r="D7"/>
       <c s="7" r="E7">
-        <v>376</v>
+        <v>311</v>
       </c>
       <c s="8" r="F7">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c s="5" t="str" r="G7"/>
-      <c s="9" r="H7">
-        <v>4</v>
-      </c>
-      <c s="10" r="I7">
+      <c s="8" r="H7">
+        <v>6</v>
+      </c>
+      <c s="9" r="I7">
         <v>0</v>
       </c>
       <c s="5" t="str" r="J7"/>
-      <c s="10" r="K7">
+      <c s="9" r="K7">
         <v>0</v>
       </c>
       <c s="5" t="str" r="L7"/>
-      <c s="10" r="M7">
+      <c s="9" r="M7">
         <v>0</v>
       </c>
       <c s="5" t="str" r="N7"/>
-      <c s="10" r="O7">
+      <c s="9" r="O7">
         <v>0</v>
       </c>
       <c s="5" t="str" r="P7"/>
-      <c s="10" r="Q7">
+      <c s="9" r="Q7">
         <v>0</v>
       </c>
       <c s="5" t="str" r="R7"/>
-      <c s="11" r="S7">
-        <v>60</v>
+      <c s="10" r="S7">
+        <v>74</v>
       </c>
       <c s="5" t="str" r="T7"/>
-      <c s="10" r="U7">
-        <v>46</v>
+      <c s="9" r="U7">
+        <v>71</v>
       </c>
       <c s="5" t="str" r="V7"/>
-      <c s="9" r="W7">
-        <v>137</v>
+      <c s="10" r="W7">
+        <v>192</v>
       </c>
       <c s="5" t="str" r="X7"/>
-      <c s="9" r="Y7">
-        <v>68</v>
+      <c s="8" r="Y7">
+        <v>96</v>
       </c>
       <c s="5" t="str" r="Z7"/>
     </row>
@@ -672,49 +672,49 @@
       <c s="4" t="str" r="C8"/>
       <c s="5" t="str" r="D8"/>
       <c s="7" r="E8">
-        <v>536</v>
+        <v>442</v>
       </c>
       <c s="11" r="F8">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c s="5" t="str" r="G8"/>
-      <c s="9" r="H8">
+      <c s="12" r="H8">
         <v>2</v>
       </c>
-      <c s="10" r="I8">
+      <c s="9" r="I8">
         <v>0</v>
       </c>
       <c s="5" t="str" r="J8"/>
-      <c s="10" r="K8">
+      <c s="9" r="K8">
         <v>0</v>
       </c>
       <c s="5" t="str" r="L8"/>
-      <c s="10" r="M8">
+      <c s="9" r="M8">
         <v>0</v>
       </c>
       <c s="5" t="str" r="N8"/>
-      <c s="10" r="O8">
+      <c s="9" r="O8">
         <v>0</v>
       </c>
       <c s="5" t="str" r="P8"/>
-      <c s="10" r="Q8">
+      <c s="9" r="Q8">
         <v>0</v>
       </c>
       <c s="5" t="str" r="R8"/>
-      <c s="12" r="S8">
-        <v>46</v>
+      <c s="13" r="S8">
+        <v>53</v>
       </c>
       <c s="5" t="str" r="T8"/>
-      <c s="10" r="U8">
-        <v>52</v>
+      <c s="9" r="U8">
+        <v>50</v>
       </c>
       <c s="5" t="str" r="V8"/>
-      <c s="9" r="W8">
-        <v>127</v>
+      <c s="12" r="W8">
+        <v>135</v>
       </c>
       <c s="5" t="str" r="X8"/>
-      <c s="9" r="Y8">
-        <v>127</v>
+      <c s="12" r="Y8">
+        <v>135</v>
       </c>
       <c s="5" t="str" r="Z8"/>
     </row>
@@ -728,49 +728,49 @@
       <c s="4" t="str" r="C9"/>
       <c s="5" t="str" r="D9"/>
       <c s="7" r="E9">
-        <v>430</v>
+        <v>391</v>
       </c>
       <c s="13" r="F9">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c s="5" t="str" r="G9"/>
-      <c s="8" r="H9">
-        <v>5</v>
-      </c>
-      <c s="10" r="I9">
+      <c s="10" r="H9">
+        <v>7</v>
+      </c>
+      <c s="9" r="I9">
         <v>0</v>
       </c>
       <c s="5" t="str" r="J9"/>
-      <c s="10" r="K9">
+      <c s="9" r="K9">
         <v>0</v>
       </c>
       <c s="5" t="str" r="L9"/>
-      <c s="10" r="M9">
+      <c s="9" r="M9">
         <v>0</v>
       </c>
       <c s="5" t="str" r="N9"/>
-      <c s="10" r="O9">
+      <c s="9" r="O9">
         <v>0</v>
       </c>
       <c s="5" t="str" r="P9"/>
-      <c s="10" r="Q9">
+      <c s="9" r="Q9">
         <v>0</v>
       </c>
       <c s="5" t="str" r="R9"/>
-      <c s="12" r="S9">
-        <v>62</v>
+      <c s="13" r="S9">
+        <v>78</v>
       </c>
       <c s="5" t="str" r="T9"/>
-      <c s="10" r="U9">
-        <v>60</v>
+      <c s="9" r="U9">
+        <v>89</v>
       </c>
       <c s="5" t="str" r="V9"/>
-      <c s="8" r="W9">
-        <v>155</v>
+      <c s="13" r="W9">
+        <v>210</v>
       </c>
       <c s="5" t="str" r="X9"/>
-      <c s="8" r="Y9">
-        <v>155</v>
+      <c s="13" r="Y9">
+        <v>210</v>
       </c>
       <c s="5" t="str" r="Z9"/>
     </row>
@@ -784,49 +784,49 @@
       <c s="4" t="str" r="C10"/>
       <c s="5" t="str" r="D10"/>
       <c s="7" r="E10">
-        <v>381</v>
-      </c>
-      <c s="12" r="F10">
-        <v>42</v>
+        <v>315</v>
+      </c>
+      <c s="11" r="F10">
+        <v>34</v>
       </c>
       <c s="5" t="str" r="G10"/>
-      <c s="13" r="H10">
-        <v>10</v>
-      </c>
-      <c s="10" r="I10">
+      <c s="10" r="H10">
+        <v>7</v>
+      </c>
+      <c s="9" r="I10">
         <v>0</v>
       </c>
       <c s="5" t="str" r="J10"/>
-      <c s="10" r="K10">
+      <c s="9" r="K10">
         <v>0</v>
       </c>
       <c s="5" t="str" r="L10"/>
-      <c s="10" r="M10">
+      <c s="9" r="M10">
         <v>0</v>
       </c>
       <c s="5" t="str" r="N10"/>
-      <c s="10" r="O10">
+      <c s="9" r="O10">
         <v>0</v>
       </c>
       <c s="5" t="str" r="P10"/>
-      <c s="10" r="Q10">
+      <c s="9" r="Q10">
         <v>0</v>
       </c>
       <c s="5" t="str" r="R10"/>
-      <c s="12" r="S10">
-        <v>64</v>
+      <c s="13" r="S10">
+        <v>68</v>
       </c>
       <c s="5" t="str" r="T10"/>
-      <c s="10" r="U10">
-        <v>72</v>
+      <c s="9" r="U10">
+        <v>73</v>
       </c>
       <c s="5" t="str" r="V10"/>
-      <c s="11" r="W10">
-        <v>179</v>
+      <c s="10" r="W10">
+        <v>174</v>
       </c>
       <c s="5" t="str" r="X10"/>
-      <c s="11" r="Y10">
-        <v>179</v>
+      <c s="10" r="Y10">
+        <v>174</v>
       </c>
       <c s="5" t="str" r="Z10"/>
     </row>
@@ -840,49 +840,49 @@
       <c s="4" t="str" r="C11"/>
       <c s="5" t="str" r="D11"/>
       <c s="7" r="E11">
-        <v>401</v>
-      </c>
-      <c s="10" r="F11">
+        <v>306</v>
+      </c>
+      <c s="9" r="F11">
         <v>0</v>
       </c>
       <c s="5" t="str" r="G11"/>
-      <c s="10" r="H11">
+      <c s="9" r="H11">
         <v>0</v>
       </c>
       <c s="13" r="I11">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c s="5" t="str" r="J11"/>
-      <c s="9" r="K11">
+      <c s="12" r="K11">
         <v>3</v>
       </c>
       <c s="5" t="str" r="L11"/>
-      <c s="9" r="M11">
+      <c s="12" r="M11">
         <v>0</v>
       </c>
       <c s="5" t="str" r="N11"/>
-      <c s="9" r="O11">
-        <v>1</v>
+      <c s="12" r="O11">
+        <v>0</v>
       </c>
       <c s="5" t="str" r="P11"/>
-      <c s="10" r="Q11">
+      <c s="9" r="Q11">
         <v>0</v>
       </c>
       <c s="5" t="str" r="R11"/>
-      <c s="12" r="S11">
-        <v>56</v>
+      <c s="13" r="S11">
+        <v>75</v>
       </c>
       <c s="5" t="str" r="T11"/>
-      <c s="10" r="U11">
-        <v>61</v>
+      <c s="9" r="U11">
+        <v>91</v>
       </c>
       <c s="5" t="str" r="V11"/>
-      <c s="9" r="W11">
-        <v>147</v>
+      <c s="13" r="W11">
+        <v>201</v>
       </c>
       <c s="5" t="str" r="X11"/>
-      <c s="9" r="Y11">
-        <v>147</v>
+      <c s="13" r="Y11">
+        <v>201</v>
       </c>
       <c s="5" t="str" r="Z11"/>
     </row>
@@ -896,49 +896,49 @@
       <c s="4" t="str" r="C12"/>
       <c s="5" t="str" r="D12"/>
       <c s="7" r="E12">
-        <v>427</v>
-      </c>
-      <c s="11" r="F12">
-        <v>43</v>
+        <v>368</v>
+      </c>
+      <c s="8" r="F12">
+        <v>37</v>
       </c>
       <c s="5" t="str" r="G12"/>
-      <c s="9" r="H12">
-        <v>4</v>
-      </c>
-      <c s="10" r="I12">
+      <c s="12" r="H12">
+        <v>3</v>
+      </c>
+      <c s="9" r="I12">
         <v>0</v>
       </c>
       <c s="5" t="str" r="J12"/>
-      <c s="10" r="K12">
+      <c s="9" r="K12">
         <v>0</v>
       </c>
       <c s="5" t="str" r="L12"/>
-      <c s="10" r="M12">
+      <c s="9" r="M12">
         <v>0</v>
       </c>
       <c s="5" t="str" r="N12"/>
-      <c s="10" r="O12">
+      <c s="9" r="O12">
         <v>0</v>
       </c>
       <c s="5" t="str" r="P12"/>
-      <c s="13" r="Q12">
-        <v>28</v>
+      <c s="10" r="Q12">
+        <v>20</v>
       </c>
       <c s="5" t="str" r="R12"/>
-      <c s="12" r="S12">
-        <v>76</v>
+      <c s="13" r="S12">
+        <v>75</v>
       </c>
       <c s="5" t="str" r="T12"/>
-      <c s="10" r="U12">
-        <v>89</v>
+      <c s="9" r="U12">
+        <v>70</v>
       </c>
       <c s="5" t="str" r="V12"/>
-      <c s="11" r="W12">
-        <v>233</v>
+      <c s="10" r="W12">
+        <v>201</v>
       </c>
       <c s="5" t="str" r="X12"/>
-      <c s="11" r="Y12">
-        <v>233</v>
+      <c s="10" r="Y12">
+        <v>201</v>
       </c>
       <c s="5" t="str" r="Z12"/>
     </row>
@@ -1047,12 +1047,12 @@
       <c s="4" t="str" r="E15"/>
       <c s="5" t="str" r="F15"/>
       <c s="19" r="G15">
-        <v>216</v>
+        <v>128</v>
       </c>
       <c s="4" t="str" r="H15"/>
       <c s="5" t="str" r="I15"/>
       <c s="20" r="J15">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c s="5" t="str" r="K15"/>
       <c s="21" r="L15">
@@ -1079,24 +1079,24 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W15"/>
-      <c s="20" r="X15">
-        <v>43</v>
+      <c s="23" r="X15">
+        <v>64</v>
       </c>
       <c s="5" t="str" r="Y15"/>
       <c s="22" r="Z15">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c s="5" t="str" r="AA15"/>
-      <c s="21" r="AB15">
-        <v>115</v>
+      <c s="23" r="AB15">
+        <v>165</v>
       </c>
       <c s="5" t="str" r="AC15"/>
       <c s="21" r="AD15">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" ht="18" customHeight="0">
-      <c s="23" t="str" r="A16"/>
+      <c s="24" t="str" r="A16"/>
       <c s="18" t="inlineStr" r="D16">
         <is>
           <t xml:space="preserve">Daypart 3</t>
@@ -1105,16 +1105,16 @@
       <c s="4" t="str" r="E16"/>
       <c s="5" t="str" r="F16"/>
       <c s="19" r="G16">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c s="4" t="str" r="H16"/>
       <c s="5" t="str" r="I16"/>
       <c s="20" r="J16">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c s="5" t="str" r="K16"/>
-      <c s="21" r="L16">
-        <v>4</v>
+      <c s="20" r="L16">
+        <v>8</v>
       </c>
       <c s="5" t="str" r="M16"/>
       <c s="22" r="N16">
@@ -1137,24 +1137,24 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W16"/>
-      <c s="24" r="X16">
-        <v>69</v>
+      <c s="23" r="X16">
+        <v>72</v>
       </c>
       <c s="5" t="str" r="Y16"/>
       <c s="22" r="Z16">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c s="5" t="str" r="AA16"/>
-      <c s="24" r="AB16">
-        <v>151</v>
+      <c s="23" r="AB16">
+        <v>203</v>
       </c>
       <c s="5" t="str" r="AC16"/>
-      <c s="21" r="AD16">
-        <v>75</v>
+      <c s="20" r="AD16">
+        <v>101</v>
       </c>
     </row>
     <row r="17" ht="18" customHeight="0">
-      <c s="23" t="str" r="A17"/>
+      <c s="24" t="str" r="A17"/>
       <c s="18" t="inlineStr" r="D17">
         <is>
           <t xml:space="preserve">Daypart 4</t>
@@ -1163,16 +1163,16 @@
       <c s="4" t="str" r="E17"/>
       <c s="5" t="str" r="F17"/>
       <c s="19" r="G17">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c s="4" t="str" r="H17"/>
       <c s="5" t="str" r="I17"/>
-      <c s="20" r="J17">
-        <v>29</v>
+      <c s="23" r="J17">
+        <v>60</v>
       </c>
       <c s="5" t="str" r="K17"/>
       <c s="20" r="L17">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c s="5" t="str" r="M17"/>
       <c s="22" r="N17">
@@ -1196,19 +1196,19 @@
       </c>
       <c s="5" t="str" r="W17"/>
       <c s="25" r="X17">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c s="5" t="str" r="Y17"/>
       <c s="22" r="Z17">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c s="5" t="str" r="AA17"/>
-      <c s="24" r="AB17">
-        <v>181</v>
+      <c s="23" r="AB17">
+        <v>231</v>
       </c>
       <c s="5" t="str" r="AC17"/>
       <c s="20" r="AD17">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" ht="18" customHeight="0">
@@ -1223,16 +1223,16 @@
       <c s="4" t="str" r="E18"/>
       <c s="5" t="str" r="F18"/>
       <c s="19" r="G18">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c s="4" t="str" r="H18"/>
       <c s="5" t="str" r="I18"/>
-      <c s="20" r="J18">
-        <v>24</v>
+      <c s="28" r="J18">
+        <v>124</v>
       </c>
       <c s="5" t="str" r="K18"/>
-      <c s="21" r="L18">
-        <v>3</v>
+      <c s="25" r="L18">
+        <v>19</v>
       </c>
       <c s="5" t="str" r="M18"/>
       <c s="22" r="N18">
@@ -1255,20 +1255,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W18"/>
-      <c s="28" r="X18">
-        <v>124</v>
+      <c s="25" r="X18">
+        <v>108</v>
       </c>
       <c s="5" t="str" r="Y18"/>
       <c s="22" r="Z18">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c s="5" t="str" r="AA18"/>
-      <c s="24" r="AB18">
-        <v>206</v>
+      <c s="23" r="AB18">
+        <v>240</v>
       </c>
       <c s="5" t="str" r="AC18"/>
       <c s="20" r="AD18">
-        <v>102</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" ht="18" customHeight="0">
@@ -1287,16 +1287,16 @@
       <c s="4" t="str" r="E19"/>
       <c s="5" t="str" r="F19"/>
       <c s="19" r="G19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c s="4" t="str" r="H19"/>
       <c s="5" t="str" r="I19"/>
-      <c s="25" r="J19">
-        <v>31</v>
+      <c s="28" r="J19">
+        <v>35</v>
       </c>
       <c s="5" t="str" r="K19"/>
       <c s="21" r="L19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M19"/>
       <c s="22" r="N19">
@@ -1320,23 +1320,23 @@
       </c>
       <c s="5" t="str" r="W19"/>
       <c s="28" r="X19">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c s="5" t="str" r="Y19"/>
       <c s="22" r="Z19">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c s="5" t="str" r="AA19"/>
       <c s="21" r="AB19">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c s="5" t="str" r="AC19"/>
       <c s="21" r="AD19">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" ht="18" customHeight="0">
-      <c s="23" t="str" r="A20"/>
+      <c s="24" t="str" r="A20"/>
       <c s="18" t="inlineStr" r="D20">
         <is>
           <t xml:space="preserve">Daypart 2</t>
@@ -1345,16 +1345,16 @@
       <c s="4" t="str" r="E20"/>
       <c s="5" t="str" r="F20"/>
       <c s="19" r="G20">
-        <v>317</v>
+        <v>172</v>
       </c>
       <c s="4" t="str" r="H20"/>
       <c s="5" t="str" r="I20"/>
-      <c s="24" r="J20">
-        <v>26</v>
+      <c s="23" r="J20">
+        <v>29</v>
       </c>
       <c s="5" t="str" r="K20"/>
       <c s="21" r="L20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M20"/>
       <c s="22" r="N20">
@@ -1377,24 +1377,24 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W20"/>
-      <c s="24" r="X20">
-        <v>36</v>
+      <c s="28" r="X20">
+        <v>46</v>
       </c>
       <c s="5" t="str" r="Y20"/>
       <c s="22" r="Z20">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c s="5" t="str" r="AA20"/>
       <c s="21" r="AB20">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c s="5" t="str" r="AC20"/>
       <c s="21" r="AD20">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" ht="18" customHeight="0">
-      <c s="23" t="str" r="A21"/>
+      <c s="24" t="str" r="A21"/>
       <c s="18" t="inlineStr" r="D21">
         <is>
           <t xml:space="preserve">Daypart 3</t>
@@ -1403,12 +1403,12 @@
       <c s="4" t="str" r="E21"/>
       <c s="5" t="str" r="F21"/>
       <c s="19" r="G21">
-        <v>132</v>
+        <v>186</v>
       </c>
       <c s="4" t="str" r="H21"/>
       <c s="5" t="str" r="I21"/>
       <c s="25" r="J21">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c s="5" t="str" r="K21"/>
       <c s="21" r="L21">
@@ -1436,23 +1436,23 @@
       </c>
       <c s="5" t="str" r="W21"/>
       <c s="28" r="X21">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c s="5" t="str" r="Y21"/>
       <c s="22" r="Z21">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c s="5" t="str" r="AA21"/>
       <c s="21" r="AB21">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c s="5" t="str" r="AC21"/>
       <c s="21" r="AD21">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" ht="18" customHeight="0">
-      <c s="23" t="str" r="A22"/>
+      <c s="24" t="str" r="A22"/>
       <c s="18" t="inlineStr" r="D22">
         <is>
           <t xml:space="preserve">Daypart 4</t>
@@ -1461,16 +1461,16 @@
       <c s="4" t="str" r="E22"/>
       <c s="5" t="str" r="F22"/>
       <c s="19" r="G22">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c s="4" t="str" r="H22"/>
       <c s="5" t="str" r="I22"/>
-      <c s="25" r="J22">
-        <v>31</v>
+      <c s="28" r="J22">
+        <v>37</v>
       </c>
       <c s="5" t="str" r="K22"/>
       <c s="21" r="L22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c s="5" t="str" r="M22"/>
       <c s="22" r="N22">
@@ -1494,19 +1494,19 @@
       </c>
       <c s="5" t="str" r="W22"/>
       <c s="28" r="X22">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c s="5" t="str" r="Y22"/>
       <c s="22" r="Z22">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c s="5" t="str" r="AA22"/>
-      <c s="21" r="AB22">
-        <v>116</v>
+      <c s="20" r="AB22">
+        <v>150</v>
       </c>
       <c s="5" t="str" r="AC22"/>
-      <c s="21" r="AD22">
-        <v>116</v>
+      <c s="20" r="AD22">
+        <v>150</v>
       </c>
     </row>
     <row r="23" ht="18" customHeight="0">
@@ -1521,16 +1521,16 @@
       <c s="4" t="str" r="E23"/>
       <c s="5" t="str" r="F23"/>
       <c s="19" r="G23">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c s="4" t="str" r="H23"/>
       <c s="5" t="str" r="I23"/>
-      <c s="28" r="J23">
-        <v>36</v>
+      <c s="20" r="J23">
+        <v>24</v>
       </c>
       <c s="5" t="str" r="K23"/>
-      <c s="20" r="L23">
-        <v>5</v>
+      <c s="21" r="L23">
+        <v>3</v>
       </c>
       <c s="5" t="str" r="M23"/>
       <c s="22" r="N23">
@@ -1554,19 +1554,19 @@
       </c>
       <c s="5" t="str" r="W23"/>
       <c s="28" r="X23">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c s="5" t="str" r="Y23"/>
       <c s="22" r="Z23">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c s="5" t="str" r="AA23"/>
       <c s="21" r="AB23">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c s="5" t="str" r="AC23"/>
       <c s="21" r="AD23">
-        <v>130</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" ht="18" customHeight="0">
@@ -1585,16 +1585,16 @@
       <c s="4" t="str" r="E24"/>
       <c s="5" t="str" r="F24"/>
       <c s="19" r="G24">
-        <v>262</v>
+        <v>148</v>
       </c>
       <c s="4" t="str" r="H24"/>
       <c s="5" t="str" r="I24"/>
-      <c s="25" r="J24">
-        <v>32</v>
+      <c s="28" r="J24">
+        <v>35</v>
       </c>
       <c s="5" t="str" r="K24"/>
-      <c s="24" r="L24">
-        <v>7</v>
+      <c s="20" r="L24">
+        <v>5</v>
       </c>
       <c s="5" t="str" r="M24"/>
       <c s="22" r="N24">
@@ -1618,23 +1618,23 @@
       </c>
       <c s="5" t="str" r="W24"/>
       <c s="28" r="X24">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c s="5" t="str" r="Y24"/>
       <c s="22" r="Z24">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c s="5" t="str" r="AA24"/>
       <c s="20" r="AB24">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c s="5" t="str" r="AC24"/>
       <c s="20" r="AD24">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" ht="18" customHeight="0">
-      <c s="23" t="str" r="A25"/>
+      <c s="24" t="str" r="A25"/>
       <c s="18" t="inlineStr" r="D25">
         <is>
           <t xml:space="preserve">Daypart 3</t>
@@ -1643,16 +1643,16 @@
       <c s="4" t="str" r="E25"/>
       <c s="5" t="str" r="F25"/>
       <c s="19" r="G25">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c s="4" t="str" r="H25"/>
       <c s="5" t="str" r="I25"/>
       <c s="28" r="J25">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c s="5" t="str" r="K25"/>
-      <c s="21" r="L25">
-        <v>3</v>
+      <c s="20" r="L25">
+        <v>6</v>
       </c>
       <c s="5" t="str" r="M25"/>
       <c s="22" r="N25">
@@ -1676,23 +1676,23 @@
       </c>
       <c s="5" t="str" r="W25"/>
       <c s="28" r="X25">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c s="5" t="str" r="Y25"/>
       <c s="22" r="Z25">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c s="5" t="str" r="AA25"/>
-      <c s="20" r="AB25">
-        <v>150</v>
+      <c s="28" r="AB25">
+        <v>232</v>
       </c>
       <c s="5" t="str" r="AC25"/>
-      <c s="20" r="AD25">
-        <v>150</v>
+      <c s="28" r="AD25">
+        <v>232</v>
       </c>
     </row>
     <row r="26" ht="18" customHeight="0">
-      <c s="23" t="str" r="A26"/>
+      <c s="24" t="str" r="A26"/>
       <c s="18" t="inlineStr" r="D26">
         <is>
           <t xml:space="preserve">Daypart 4</t>
@@ -1701,16 +1701,16 @@
       <c s="4" t="str" r="E26"/>
       <c s="5" t="str" r="F26"/>
       <c s="19" r="G26">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c s="4" t="str" r="H26"/>
       <c s="5" t="str" r="I26"/>
       <c s="28" r="J26">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c s="5" t="str" r="K26"/>
-      <c s="21" r="L26">
-        <v>4</v>
+      <c s="28" r="L26">
+        <v>14</v>
       </c>
       <c s="5" t="str" r="M26"/>
       <c s="22" r="N26">
@@ -1734,19 +1734,19 @@
       </c>
       <c s="5" t="str" r="W26"/>
       <c s="28" r="X26">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c s="5" t="str" r="Y26"/>
       <c s="22" r="Z26">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c s="5" t="str" r="AA26"/>
-      <c s="24" r="AB26">
-        <v>177</v>
+      <c s="28" r="AB26">
+        <v>282</v>
       </c>
       <c s="5" t="str" r="AC26"/>
-      <c s="24" r="AD26">
-        <v>177</v>
+      <c s="28" r="AD26">
+        <v>282</v>
       </c>
     </row>
     <row r="27" ht="18" customHeight="0">
@@ -1761,16 +1761,16 @@
       <c s="4" t="str" r="E27"/>
       <c s="5" t="str" r="F27"/>
       <c s="19" r="G27">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c s="4" t="str" r="H27"/>
       <c s="5" t="str" r="I27"/>
-      <c s="25" r="J27">
-        <v>34</v>
+      <c s="28" r="J27">
+        <v>47</v>
       </c>
       <c s="5" t="str" r="K27"/>
       <c s="21" r="L27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c s="5" t="str" r="M27"/>
       <c s="22" r="N27">
@@ -1794,19 +1794,19 @@
       </c>
       <c s="5" t="str" r="W27"/>
       <c s="28" r="X27">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c s="5" t="str" r="Y27"/>
       <c s="22" r="Z27">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c s="5" t="str" r="AA27"/>
-      <c s="21" r="AB27">
-        <v>120</v>
+      <c s="28" r="AB27">
+        <v>203</v>
       </c>
       <c s="5" t="str" r="AC27"/>
-      <c s="21" r="AD27">
-        <v>120</v>
+      <c s="28" r="AD27">
+        <v>203</v>
       </c>
     </row>
     <row r="28" ht="18" customHeight="0">
@@ -1825,16 +1825,16 @@
       <c s="4" t="str" r="E28"/>
       <c s="5" t="str" r="F28"/>
       <c s="19" r="G28">
-        <v>222</v>
+        <v>135</v>
       </c>
       <c s="4" t="str" r="H28"/>
       <c s="5" t="str" r="I28"/>
-      <c s="28" r="J28">
-        <v>35</v>
+      <c s="20" r="J28">
+        <v>22</v>
       </c>
       <c s="5" t="str" r="K28"/>
-      <c s="24" r="L28">
-        <v>7</v>
+      <c s="21" r="L28">
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M28"/>
       <c s="22" r="N28">
@@ -1858,23 +1858,23 @@
       </c>
       <c s="5" t="str" r="W28"/>
       <c s="28" r="X28">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c s="5" t="str" r="Y28"/>
       <c s="22" r="Z28">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c s="5" t="str" r="AA28"/>
-      <c s="25" r="AB28">
-        <v>181</v>
+      <c s="21" r="AB28">
+        <v>128</v>
       </c>
       <c s="5" t="str" r="AC28"/>
-      <c s="25" r="AD28">
-        <v>181</v>
+      <c s="21" r="AD28">
+        <v>128</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="0">
-      <c s="23" t="str" r="A29"/>
+      <c s="24" t="str" r="A29"/>
       <c s="18" t="inlineStr" r="D29">
         <is>
           <t xml:space="preserve">Daypart 3</t>
@@ -1883,16 +1883,16 @@
       <c s="4" t="str" r="E29"/>
       <c s="5" t="str" r="F29"/>
       <c s="19" r="G29">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c s="4" t="str" r="H29"/>
       <c s="5" t="str" r="I29"/>
       <c s="28" r="J29">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c s="5" t="str" r="K29"/>
       <c s="28" r="L29">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c s="5" t="str" r="M29"/>
       <c s="22" r="N29">
@@ -1916,23 +1916,23 @@
       </c>
       <c s="5" t="str" r="W29"/>
       <c s="28" r="X29">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c s="5" t="str" r="Y29"/>
       <c s="22" r="Z29">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c s="5" t="str" r="AA29"/>
       <c s="28" r="AB29">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c s="5" t="str" r="AC29"/>
       <c s="28" r="AD29">
-        <v>197</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" ht="18" customHeight="0">
-      <c s="23" t="str" r="A30"/>
+      <c s="24" t="str" r="A30"/>
       <c s="18" t="inlineStr" r="D30">
         <is>
           <t xml:space="preserve">Daypart 4</t>
@@ -1941,16 +1941,16 @@
       <c s="4" t="str" r="E30"/>
       <c s="5" t="str" r="F30"/>
       <c s="19" r="G30">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c s="4" t="str" r="H30"/>
       <c s="5" t="str" r="I30"/>
       <c s="28" r="J30">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c s="5" t="str" r="K30"/>
-      <c s="28" r="L30">
-        <v>14</v>
+      <c s="21" r="L30">
+        <v>4</v>
       </c>
       <c s="5" t="str" r="M30"/>
       <c s="22" r="N30">
@@ -1974,19 +1974,19 @@
       </c>
       <c s="5" t="str" r="W30"/>
       <c s="28" r="X30">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c s="5" t="str" r="Y30"/>
       <c s="22" r="Z30">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c s="5" t="str" r="AA30"/>
-      <c s="20" r="AB30">
-        <v>155</v>
+      <c s="28" r="AB30">
+        <v>211</v>
       </c>
       <c s="5" t="str" r="AC30"/>
-      <c s="20" r="AD30">
-        <v>155</v>
+      <c s="28" r="AD30">
+        <v>211</v>
       </c>
     </row>
     <row r="31" ht="18" customHeight="0">
@@ -2001,16 +2001,16 @@
       <c s="4" t="str" r="E31"/>
       <c s="5" t="str" r="F31"/>
       <c s="19" r="G31">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c s="4" t="str" r="H31"/>
       <c s="5" t="str" r="I31"/>
       <c s="28" r="J31">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c s="5" t="str" r="K31"/>
-      <c s="20" r="L31">
-        <v>6</v>
+      <c s="25" r="L31">
+        <v>11</v>
       </c>
       <c s="5" t="str" r="M31"/>
       <c s="22" r="N31">
@@ -2034,19 +2034,19 @@
       </c>
       <c s="5" t="str" r="W31"/>
       <c s="28" r="X31">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c s="5" t="str" r="Y31"/>
       <c s="22" r="Z31">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c s="5" t="str" r="AA31"/>
-      <c s="21" r="AB31">
-        <v>124</v>
+      <c s="20" r="AB31">
+        <v>156</v>
       </c>
       <c s="5" t="str" r="AC31"/>
-      <c s="21" r="AD31">
-        <v>124</v>
+      <c s="20" r="AD31">
+        <v>156</v>
       </c>
     </row>
     <row r="32" ht="18" customHeight="0">
@@ -2065,7 +2065,7 @@
       <c s="4" t="str" r="E32"/>
       <c s="5" t="str" r="F32"/>
       <c s="19" r="G32">
-        <v>244</v>
+        <v>115</v>
       </c>
       <c s="4" t="str" r="H32"/>
       <c s="5" t="str" r="I32"/>
@@ -2077,20 +2077,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="M32"/>
-      <c s="25" r="N32">
-        <v>31</v>
+      <c s="23" r="N32">
+        <v>28</v>
       </c>
       <c s="5" t="str" r="O32"/>
       <c s="21" r="P32">
         <v>2</v>
       </c>
       <c s="5" t="str" r="Q32"/>
-      <c s="21" r="R32">
+      <c s="22" r="R32">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S32"/>
-      <c s="21" r="T32">
-        <v>2</v>
+      <c s="22" r="T32">
+        <v>0</v>
       </c>
       <c s="5" t="str" r="U32"/>
       <c s="22" r="V32">
@@ -2098,23 +2098,23 @@
       </c>
       <c s="5" t="str" r="W32"/>
       <c s="28" r="X32">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c s="5" t="str" r="Y32"/>
       <c s="22" r="Z32">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c s="5" t="str" r="AA32"/>
-      <c s="20" r="AB32">
-        <v>155</v>
+      <c s="25" r="AB32">
+        <v>184</v>
       </c>
       <c s="5" t="str" r="AC32"/>
-      <c s="20" r="AD32">
-        <v>155</v>
+      <c s="25" r="AD32">
+        <v>184</v>
       </c>
     </row>
     <row r="33" ht="18" customHeight="0">
-      <c s="23" t="str" r="A33"/>
+      <c s="24" t="str" r="A33"/>
       <c s="18" t="inlineStr" r="D33">
         <is>
           <t xml:space="preserve">Daypart 3</t>
@@ -2123,7 +2123,7 @@
       <c s="4" t="str" r="E33"/>
       <c s="5" t="str" r="F33"/>
       <c s="19" r="G33">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c s="4" t="str" r="H33"/>
       <c s="5" t="str" r="I33"/>
@@ -2136,19 +2136,19 @@
       </c>
       <c s="5" t="str" r="M33"/>
       <c s="28" r="N33">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c s="5" t="str" r="O33"/>
       <c s="21" r="P33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c s="5" t="str" r="Q33"/>
       <c s="21" r="R33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c s="5" t="str" r="S33"/>
       <c s="21" r="T33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c s="5" t="str" r="U33"/>
       <c s="22" r="V33">
@@ -2156,23 +2156,23 @@
       </c>
       <c s="5" t="str" r="W33"/>
       <c s="28" r="X33">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c s="5" t="str" r="Y33"/>
       <c s="22" r="Z33">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c s="5" t="str" r="AA33"/>
-      <c s="21" r="AB33">
-        <v>148</v>
+      <c s="28" r="AB33">
+        <v>236</v>
       </c>
       <c s="5" t="str" r="AC33"/>
-      <c s="21" r="AD33">
-        <v>148</v>
+      <c s="28" r="AD33">
+        <v>236</v>
       </c>
     </row>
     <row r="34" ht="18" customHeight="0">
-      <c s="23" t="str" r="A34"/>
+      <c s="24" t="str" r="A34"/>
       <c s="18" t="inlineStr" r="D34">
         <is>
           <t xml:space="preserve">Daypart 4</t>
@@ -2181,7 +2181,7 @@
       <c s="4" t="str" r="E34"/>
       <c s="5" t="str" r="F34"/>
       <c s="19" r="G34">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c s="4" t="str" r="H34"/>
       <c s="5" t="str" r="I34"/>
@@ -2193,12 +2193,12 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="M34"/>
-      <c s="24" r="N34">
-        <v>29</v>
+      <c s="28" r="N34">
+        <v>43</v>
       </c>
       <c s="5" t="str" r="O34"/>
-      <c s="21" r="P34">
-        <v>2</v>
+      <c s="20" r="P34">
+        <v>6</v>
       </c>
       <c s="5" t="str" r="Q34"/>
       <c s="22" r="R34">
@@ -2214,19 +2214,19 @@
       </c>
       <c s="5" t="str" r="W34"/>
       <c s="28" r="X34">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c s="5" t="str" r="Y34"/>
       <c s="22" r="Z34">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c s="5" t="str" r="AA34"/>
       <c s="21" r="AB34">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c s="5" t="str" r="AC34"/>
       <c s="21" r="AD34">
-        <v>124</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" ht="18" customHeight="0">
@@ -2241,7 +2241,7 @@
       <c s="4" t="str" r="E35"/>
       <c s="5" t="str" r="F35"/>
       <c s="19" r="G35">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c s="4" t="str" r="H35"/>
       <c s="5" t="str" r="I35"/>
@@ -2258,14 +2258,14 @@
       </c>
       <c s="5" t="str" r="O35"/>
       <c s="21" r="P35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c s="5" t="str" r="Q35"/>
-      <c s="21" r="R35">
+      <c s="22" r="R35">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S35"/>
-      <c s="21" r="T35">
+      <c s="22" r="T35">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U35"/>
@@ -2274,19 +2274,19 @@
       </c>
       <c s="5" t="str" r="W35"/>
       <c s="28" r="X35">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c s="5" t="str" r="Y35"/>
       <c s="22" r="Z35">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c s="5" t="str" r="AA35"/>
-      <c s="21" r="AB35">
-        <v>99</v>
+      <c s="23" r="AB35">
+        <v>172</v>
       </c>
       <c s="5" t="str" r="AC35"/>
-      <c s="21" r="AD35">
-        <v>99</v>
+      <c s="23" r="AD35">
+        <v>172</v>
       </c>
     </row>
     <row r="36" ht="18" customHeight="0">
@@ -2305,16 +2305,16 @@
       <c s="4" t="str" r="E36"/>
       <c s="5" t="str" r="F36"/>
       <c s="19" r="G36">
-        <v>224</v>
+        <v>150</v>
       </c>
       <c s="4" t="str" r="H36"/>
       <c s="5" t="str" r="I36"/>
-      <c s="24" r="J36">
-        <v>45</v>
+      <c s="21" r="J36">
+        <v>28</v>
       </c>
       <c s="5" t="str" r="K36"/>
       <c s="21" r="L36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M36"/>
       <c s="22" r="N36">
@@ -2333,28 +2333,28 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="U36"/>
-      <c s="28" r="V36">
-        <v>33</v>
+      <c s="21" r="V36">
+        <v>13</v>
       </c>
       <c s="5" t="str" r="W36"/>
       <c s="28" r="X36">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c s="5" t="str" r="Y36"/>
       <c s="22" r="Z36">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c s="5" t="str" r="AA36"/>
-      <c s="25" r="AB36">
-        <v>248</v>
+      <c s="20" r="AB36">
+        <v>154</v>
       </c>
       <c s="5" t="str" r="AC36"/>
-      <c s="25" r="AD36">
-        <v>248</v>
+      <c s="20" r="AD36">
+        <v>154</v>
       </c>
     </row>
     <row r="37" ht="18" customHeight="0">
-      <c s="23" t="str" r="A37"/>
+      <c s="24" t="str" r="A37"/>
       <c s="18" t="inlineStr" r="D37">
         <is>
           <t xml:space="preserve">Daypart 3</t>
@@ -2363,16 +2363,16 @@
       <c s="4" t="str" r="E37"/>
       <c s="5" t="str" r="F37"/>
       <c s="19" r="G37">
-        <v>115</v>
+        <v>145</v>
       </c>
       <c s="4" t="str" r="H37"/>
       <c s="5" t="str" r="I37"/>
-      <c s="24" r="J37">
-        <v>43</v>
+      <c s="23" r="J37">
+        <v>41</v>
       </c>
       <c s="5" t="str" r="K37"/>
       <c s="21" r="L37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c s="5" t="str" r="M37"/>
       <c s="22" r="N37">
@@ -2392,27 +2392,27 @@
       </c>
       <c s="5" t="str" r="U37"/>
       <c s="25" r="V37">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c s="5" t="str" r="W37"/>
       <c s="28" r="X37">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c s="5" t="str" r="Y37"/>
       <c s="22" r="Z37">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c s="5" t="str" r="AA37"/>
-      <c s="24" r="AB37">
-        <v>237</v>
+      <c s="23" r="AB37">
+        <v>233</v>
       </c>
       <c s="5" t="str" r="AC37"/>
-      <c s="24" r="AD37">
-        <v>237</v>
+      <c s="23" r="AD37">
+        <v>233</v>
       </c>
     </row>
     <row r="38" ht="18" customHeight="0">
-      <c s="23" t="str" r="A38"/>
+      <c s="24" t="str" r="A38"/>
       <c s="18" t="inlineStr" r="D38">
         <is>
           <t xml:space="preserve">Daypart 4</t>
@@ -2421,16 +2421,16 @@
       <c s="4" t="str" r="E38"/>
       <c s="5" t="str" r="F38"/>
       <c s="19" r="G38">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c s="4" t="str" r="H38"/>
       <c s="5" t="str" r="I38"/>
-      <c s="20" r="J38">
-        <v>35</v>
+      <c s="25" r="J38">
+        <v>52</v>
       </c>
       <c s="5" t="str" r="K38"/>
       <c s="20" r="L38">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c s="5" t="str" r="M38"/>
       <c s="22" r="N38">
@@ -2449,24 +2449,24 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="U38"/>
-      <c s="21" r="V38">
-        <v>13</v>
+      <c s="28" r="V38">
+        <v>30</v>
       </c>
       <c s="5" t="str" r="W38"/>
       <c s="28" r="X38">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c s="5" t="str" r="Y38"/>
       <c s="22" r="Z38">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c s="5" t="str" r="AA38"/>
-      <c s="20" r="AB38">
-        <v>170</v>
+      <c s="25" r="AB38">
+        <v>247</v>
       </c>
       <c s="5" t="str" r="AC38"/>
-      <c s="20" r="AD38">
-        <v>170</v>
+      <c s="25" r="AD38">
+        <v>247</v>
       </c>
     </row>
     <row r="39" ht="18" customHeight="0">
@@ -2481,16 +2481,16 @@
       <c s="4" t="str" r="E39"/>
       <c s="5" t="str" r="F39"/>
       <c s="19" r="G39">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c s="4" t="str" r="H39"/>
       <c s="5" t="str" r="I39"/>
-      <c s="24" r="J39">
-        <v>41</v>
+      <c s="20" r="J39">
+        <v>38</v>
       </c>
       <c s="5" t="str" r="K39"/>
       <c s="20" r="L39">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c s="5" t="str" r="M39"/>
       <c s="22" r="N39">
@@ -2509,24 +2509,24 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="U39"/>
-      <c s="25" r="V39">
-        <v>28</v>
+      <c s="21" r="V39">
+        <v>2</v>
       </c>
       <c s="5" t="str" r="W39"/>
       <c s="28" r="X39">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c s="5" t="str" r="Y39"/>
       <c s="22" r="Z39">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c s="5" t="str" r="AA39"/>
-      <c s="24" r="AB39">
-        <v>233</v>
+      <c s="20" r="AB39">
+        <v>173</v>
       </c>
       <c s="5" t="str" r="AC39"/>
-      <c s="24" r="AD39">
-        <v>233</v>
+      <c s="20" r="AD39">
+        <v>173</v>
       </c>
     </row>
     <row r="40" ht="0.05" customHeight="1"/>
@@ -2935,7 +2935,7 @@
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.95" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;L&amp;"Segoe UI,Italic"&amp;9 Print Date &amp;&amp; Time: 11/13/2025 12:30:58 PM 
+    <oddFooter>&amp;L&amp;"Segoe UI,Italic"&amp;9 Print Date &amp;&amp; Time: 12/1/2025 12:39:06 PM 
 &amp;"-,Italic"Page Number:  &amp;P </oddFooter>
   </headerFooter>
   <drawing r:id="rId7"/>

</xml_diff>

<commit_message>
update on downloading data from gmail
</commit_message>
<xml_diff>
--- a/data/hme/raw/hme_report.xlsx
+++ b/data/hme/raw/hme_report.xlsx
@@ -265,7 +265,7 @@
   <cellStyleXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf applyFont="1" applyFill="1" applyBorder="1" numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
@@ -303,9 +303,6 @@
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="82" fontId="7" fillId="7" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="82" fontId="7" fillId="8" borderId="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="0" fontId="4" fillId="2" borderId="4">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
@@ -333,13 +330,10 @@
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="10" fillId="3" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="6" borderId="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="0" fontId="1" fillId="3" borderId="6">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="8" borderId="1">
+    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="6" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="0" fontId="1" fillId="3" borderId="7">
@@ -349,6 +343,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="7" borderId="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="8" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -520,7 +517,7 @@
     <row r="3" ht="18.15" customHeight="1">
       <c s="2" t="inlineStr" r="C3">
         <is>
-          <t xml:space="preserve">Day: 02/04/2026</t>
+          <t xml:space="preserve">Day: 02/05/2026</t>
         </is>
       </c>
     </row>
@@ -616,14 +613,14 @@
       <c s="4" t="str" r="C7"/>
       <c s="5" t="str" r="D7"/>
       <c s="7" r="E7">
-        <v>352</v>
+        <v>379</v>
       </c>
       <c s="8" r="F7">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c s="5" t="str" r="G7"/>
       <c s="9" r="H7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c s="10" r="I7">
         <v>0</v>
@@ -645,20 +642,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="R7"/>
-      <c s="11" r="S7">
-        <v>63</v>
+      <c s="8" r="S7">
+        <v>51</v>
       </c>
       <c s="5" t="str" r="T7"/>
       <c s="10" r="U7">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c s="5" t="str" r="V7"/>
       <c s="9" r="W7">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c s="5" t="str" r="X7"/>
       <c s="9" r="Y7">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c s="5" t="str" r="Z7"/>
     </row>
@@ -672,14 +669,14 @@
       <c s="4" t="str" r="C8"/>
       <c s="5" t="str" r="D8"/>
       <c s="7" r="E8">
-        <v>554</v>
+        <v>497</v>
       </c>
       <c s="11" r="F8">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c s="5" t="str" r="G8"/>
-      <c s="8" r="H8">
-        <v>5</v>
+      <c s="9" r="H8">
+        <v>2</v>
       </c>
       <c s="10" r="I8">
         <v>0</v>
@@ -702,19 +699,19 @@
       </c>
       <c s="5" t="str" r="R8"/>
       <c s="12" r="S8">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c s="5" t="str" r="T8"/>
       <c s="10" r="U8">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c s="5" t="str" r="V8"/>
       <c s="9" r="W8">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c s="5" t="str" r="X8"/>
       <c s="9" r="Y8">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c s="5" t="str" r="Z8"/>
     </row>
@@ -728,14 +725,14 @@
       <c s="4" t="str" r="C9"/>
       <c s="5" t="str" r="D9"/>
       <c s="7" r="E9">
-        <v>416</v>
+        <v>441</v>
       </c>
       <c s="12" r="F9">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c s="5" t="str" r="G9"/>
-      <c s="11" r="H9">
-        <v>7</v>
+      <c s="8" r="H9">
+        <v>6</v>
       </c>
       <c s="10" r="I9">
         <v>0</v>
@@ -758,19 +755,19 @@
       </c>
       <c s="5" t="str" r="R9"/>
       <c s="12" r="S9">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c s="5" t="str" r="T9"/>
       <c s="10" r="U9">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c s="5" t="str" r="V9"/>
       <c s="8" r="W9">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c s="5" t="str" r="X9"/>
       <c s="8" r="Y9">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c s="5" t="str" r="Z9"/>
     </row>
@@ -784,14 +781,14 @@
       <c s="4" t="str" r="C10"/>
       <c s="5" t="str" r="D10"/>
       <c s="7" r="E10">
-        <v>370</v>
+        <v>342</v>
       </c>
       <c s="12" r="F10">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c s="5" t="str" r="G10"/>
       <c s="8" r="H10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c s="10" r="I10">
         <v>0</v>
@@ -814,19 +811,19 @@
       </c>
       <c s="5" t="str" r="R10"/>
       <c s="12" r="S10">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c s="5" t="str" r="T10"/>
       <c s="10" r="U10">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c s="5" t="str" r="V10"/>
-      <c s="13" r="W10">
-        <v>188</v>
+      <c s="11" r="W10">
+        <v>170</v>
       </c>
       <c s="5" t="str" r="X10"/>
-      <c s="13" r="Y10">
-        <v>188</v>
+      <c s="11" r="Y10">
+        <v>170</v>
       </c>
       <c s="5" t="str" r="Z10"/>
     </row>
@@ -840,14 +837,14 @@
       <c s="4" t="str" r="C11"/>
       <c s="5" t="str" r="D11"/>
       <c s="7" r="E11">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c s="8" r="F11">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c s="5" t="str" r="G11"/>
       <c s="9" r="H11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c s="10" r="I11">
         <v>0</v>
@@ -870,19 +867,19 @@
       </c>
       <c s="5" t="str" r="R11"/>
       <c s="12" r="S11">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c s="5" t="str" r="T11"/>
       <c s="10" r="U11">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c s="5" t="str" r="V11"/>
-      <c s="9" r="W11">
-        <v>104</v>
+      <c s="8" r="W11">
+        <v>120</v>
       </c>
       <c s="5" t="str" r="X11"/>
       <c s="8" r="Y11">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c s="5" t="str" r="Z11"/>
     </row>
@@ -896,7 +893,7 @@
       <c s="4" t="str" r="C12"/>
       <c s="5" t="str" r="D12"/>
       <c s="7" r="E12">
-        <v>400</v>
+        <v>363</v>
       </c>
       <c s="10" r="F12">
         <v>0</v>
@@ -905,12 +902,12 @@
       <c s="10" r="H12">
         <v>0</v>
       </c>
-      <c s="13" r="I12">
-        <v>30</v>
+      <c s="11" r="I12">
+        <v>29</v>
       </c>
       <c s="5" t="str" r="J12"/>
       <c s="9" r="K12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c s="5" t="str" r="L12"/>
       <c s="9" r="M12">
@@ -918,7 +915,7 @@
       </c>
       <c s="5" t="str" r="N12"/>
       <c s="9" r="O12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c s="5" t="str" r="P12"/>
       <c s="10" r="Q12">
@@ -926,11 +923,11 @@
       </c>
       <c s="5" t="str" r="R12"/>
       <c s="12" r="S12">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c s="5" t="str" r="T12"/>
       <c s="10" r="U12">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c s="5" t="str" r="V12"/>
       <c s="9" r="W12">
@@ -952,14 +949,14 @@
       <c s="4" t="str" r="C13"/>
       <c s="5" t="str" r="D13"/>
       <c s="7" r="E13">
-        <v>348</v>
-      </c>
-      <c s="13" r="F13">
-        <v>54</v>
+        <v>410</v>
+      </c>
+      <c s="8" r="F13">
+        <v>30</v>
       </c>
       <c s="5" t="str" r="G13"/>
-      <c s="8" r="H13">
-        <v>6</v>
+      <c s="9" r="H13">
+        <v>2</v>
       </c>
       <c s="10" r="I13">
         <v>0</v>
@@ -977,30 +974,30 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="P13"/>
-      <c s="8" r="Q13">
-        <v>16</v>
+      <c s="9" r="Q13">
+        <v>13</v>
       </c>
       <c s="5" t="str" r="R13"/>
       <c s="12" r="S13">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c s="5" t="str" r="T13"/>
       <c s="10" r="U13">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c s="5" t="str" r="V13"/>
-      <c s="11" r="W13">
-        <v>209</v>
+      <c s="9" r="W13">
+        <v>149</v>
       </c>
       <c s="5" t="str" r="X13"/>
-      <c s="11" r="Y13">
-        <v>209</v>
+      <c s="9" r="Y13">
+        <v>149</v>
       </c>
       <c s="5" t="str" r="Z13"/>
     </row>
     <row r="14" ht="4.95" customHeight="1"/>
     <row r="15" ht="32.25" customHeight="0">
-      <c s="14" t="inlineStr" r="A15">
+      <c s="13" t="inlineStr" r="A15">
         <is>
           <t xml:space="preserve">Group / Store</t>
         </is>
@@ -1021,1808 +1018,1808 @@
       </c>
       <c s="4" t="str" r="H15"/>
       <c s="5" t="str" r="I15"/>
-      <c s="15" t="inlineStr" r="J15">
+      <c s="14" t="inlineStr" r="J15">
         <is>
           <t xml:space="preserve">Menu Board</t>
         </is>
       </c>
       <c s="5" t="str" r="K15"/>
-      <c s="15" t="inlineStr" r="L15">
+      <c s="14" t="inlineStr" r="L15">
         <is>
           <t xml:space="preserve">Greet</t>
         </is>
       </c>
       <c s="5" t="str" r="M15"/>
-      <c s="15" t="inlineStr" r="N15">
+      <c s="14" t="inlineStr" r="N15">
         <is>
           <t xml:space="preserve">Menu 1</t>
         </is>
       </c>
       <c s="5" t="str" r="O15"/>
-      <c s="15" t="inlineStr" r="P15">
+      <c s="14" t="inlineStr" r="P15">
         <is>
           <t xml:space="preserve">Greet 1</t>
         </is>
       </c>
       <c s="5" t="str" r="Q15"/>
-      <c s="15" t="inlineStr" r="R15">
+      <c s="14" t="inlineStr" r="R15">
         <is>
           <t xml:space="preserve">Menu 2</t>
         </is>
       </c>
       <c s="5" t="str" r="S15"/>
-      <c s="15" t="inlineStr" r="T15">
+      <c s="14" t="inlineStr" r="T15">
         <is>
           <t xml:space="preserve">Greet 2</t>
         </is>
       </c>
       <c s="5" t="str" r="U15"/>
-      <c s="15" t="inlineStr" r="V15">
+      <c s="14" t="inlineStr" r="V15">
         <is>
           <t xml:space="preserve">Cashier</t>
         </is>
       </c>
       <c s="5" t="str" r="W15"/>
-      <c s="15" t="inlineStr" r="X15">
+      <c s="14" t="inlineStr" r="X15">
         <is>
           <t xml:space="preserve">Service</t>
         </is>
       </c>
       <c s="5" t="str" r="Y15"/>
-      <c s="15" t="inlineStr" r="Z15">
+      <c s="14" t="inlineStr" r="Z15">
         <is>
           <t xml:space="preserve">Lane Queue</t>
         </is>
       </c>
       <c s="5" t="str" r="AA15"/>
-      <c s="15" t="inlineStr" r="AB15">
+      <c s="14" t="inlineStr" r="AB15">
         <is>
           <t xml:space="preserve">Lane Total</t>
         </is>
       </c>
       <c s="5" t="str" r="AC15"/>
-      <c s="15" t="inlineStr" r="AD15">
+      <c s="14" t="inlineStr" r="AD15">
         <is>
           <t xml:space="preserve">Lane Total 2</t>
         </is>
       </c>
     </row>
     <row r="16" ht="18" customHeight="0">
-      <c s="16" t="inlineStr" r="A16">
+      <c s="15" t="inlineStr" r="A16">
         <is>
           <t xml:space="preserve">343939 Mt Joy</t>
         </is>
       </c>
-      <c s="17" t="str" r="B16"/>
-      <c s="17" t="str" r="C16"/>
-      <c s="18" t="inlineStr" r="D16">
+      <c s="16" t="str" r="B16"/>
+      <c s="16" t="str" r="C16"/>
+      <c s="17" t="inlineStr" r="D16">
         <is>
           <t xml:space="preserve">Daypart 2</t>
         </is>
       </c>
       <c s="4" t="str" r="E16"/>
       <c s="5" t="str" r="F16"/>
-      <c s="19" r="G16">
+      <c s="18" r="G16">
         <v>208</v>
       </c>
       <c s="4" t="str" r="H16"/>
       <c s="5" t="str" r="I16"/>
-      <c s="20" r="J16">
-        <v>31</v>
+      <c s="19" r="J16">
+        <v>28</v>
       </c>
       <c s="5" t="str" r="K16"/>
-      <c s="21" r="L16">
-        <v>4</v>
+      <c s="20" r="L16">
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M16"/>
-      <c s="22" r="N16">
+      <c s="21" r="N16">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O16"/>
-      <c s="22" r="P16">
+      <c s="21" r="P16">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q16"/>
-      <c s="22" r="R16">
+      <c s="21" r="R16">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S16"/>
-      <c s="22" r="T16">
+      <c s="21" r="T16">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U16"/>
-      <c s="22" r="V16">
+      <c s="21" r="V16">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W16"/>
-      <c s="20" r="X16">
-        <v>55</v>
+      <c s="19" r="X16">
+        <v>44</v>
       </c>
       <c s="5" t="str" r="Y16"/>
-      <c s="22" r="Z16">
-        <v>73</v>
+      <c s="21" r="Z16">
+        <v>47</v>
       </c>
       <c s="5" t="str" r="AA16"/>
-      <c s="23" r="AB16">
-        <v>160</v>
+      <c s="20" r="AB16">
+        <v>119</v>
       </c>
       <c s="5" t="str" r="AC16"/>
-      <c s="21" r="AD16">
-        <v>79</v>
+      <c s="20" r="AD16">
+        <v>59</v>
       </c>
     </row>
     <row r="17" ht="18" customHeight="0">
-      <c s="24" t="str" r="A17"/>
-      <c s="18" t="inlineStr" r="D17">
+      <c s="22" t="str" r="A17"/>
+      <c s="17" t="inlineStr" r="D17">
         <is>
           <t xml:space="preserve">Daypart 3</t>
         </is>
       </c>
       <c s="4" t="str" r="E17"/>
       <c s="5" t="str" r="F17"/>
-      <c s="19" r="G17">
-        <v>79</v>
+      <c s="18" r="G17">
+        <v>103</v>
       </c>
       <c s="4" t="str" r="H17"/>
       <c s="5" t="str" r="I17"/>
-      <c s="20" r="J17">
-        <v>30</v>
+      <c s="19" r="J17">
+        <v>22</v>
       </c>
       <c s="5" t="str" r="K17"/>
-      <c s="21" r="L17">
-        <v>4</v>
+      <c s="20" r="L17">
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M17"/>
-      <c s="22" r="N17">
+      <c s="21" r="N17">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O17"/>
-      <c s="22" r="P17">
+      <c s="21" r="P17">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q17"/>
-      <c s="22" r="R17">
+      <c s="21" r="R17">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S17"/>
-      <c s="22" r="T17">
+      <c s="21" r="T17">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U17"/>
-      <c s="22" r="V17">
+      <c s="21" r="V17">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W17"/>
-      <c s="23" r="X17">
-        <v>60</v>
+      <c s="19" r="X17">
+        <v>51</v>
       </c>
       <c s="5" t="str" r="Y17"/>
-      <c s="22" r="Z17">
-        <v>22</v>
+      <c s="21" r="Z17">
+        <v>29</v>
       </c>
       <c s="5" t="str" r="AA17"/>
-      <c s="21" r="AB17">
-        <v>113</v>
+      <c s="20" r="AB17">
+        <v>103</v>
       </c>
       <c s="5" t="str" r="AC17"/>
-      <c s="21" r="AD17">
-        <v>56</v>
+      <c s="20" r="AD17">
+        <v>51</v>
       </c>
     </row>
     <row r="18" ht="18" customHeight="0">
-      <c s="24" t="str" r="A18"/>
-      <c s="18" t="inlineStr" r="D18">
+      <c s="22" t="str" r="A18"/>
+      <c s="17" t="inlineStr" r="D18">
         <is>
           <t xml:space="preserve">Daypart 4</t>
         </is>
       </c>
       <c s="4" t="str" r="E18"/>
       <c s="5" t="str" r="F18"/>
-      <c s="19" r="G18">
-        <v>55</v>
+      <c s="18" r="G18">
+        <v>56</v>
       </c>
       <c s="4" t="str" r="H18"/>
       <c s="5" t="str" r="I18"/>
-      <c s="20" r="J18">
-        <v>27</v>
+      <c s="19" r="J18">
+        <v>22</v>
       </c>
       <c s="5" t="str" r="K18"/>
-      <c s="21" r="L18">
+      <c s="20" r="L18">
         <v>2</v>
       </c>
       <c s="5" t="str" r="M18"/>
-      <c s="22" r="N18">
+      <c s="21" r="N18">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O18"/>
-      <c s="22" r="P18">
+      <c s="21" r="P18">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q18"/>
-      <c s="22" r="R18">
+      <c s="21" r="R18">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S18"/>
-      <c s="22" r="T18">
+      <c s="21" r="T18">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U18"/>
-      <c s="22" r="V18">
+      <c s="21" r="V18">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W18"/>
-      <c s="25" r="X18">
-        <v>90</v>
+      <c s="23" r="X18">
+        <v>71</v>
       </c>
       <c s="5" t="str" r="Y18"/>
-      <c s="22" r="Z18">
-        <v>48</v>
+      <c s="21" r="Z18">
+        <v>14</v>
       </c>
       <c s="5" t="str" r="AA18"/>
-      <c s="23" r="AB18">
-        <v>166</v>
+      <c s="20" r="AB18">
+        <v>108</v>
       </c>
       <c s="5" t="str" r="AC18"/>
-      <c s="21" r="AD18">
-        <v>83</v>
+      <c s="20" r="AD18">
+        <v>54</v>
       </c>
     </row>
     <row r="19" ht="18" customHeight="0">
-      <c s="26" t="str" r="A19"/>
-      <c s="27" t="str" r="B19"/>
-      <c s="27" t="str" r="C19"/>
-      <c s="18" t="inlineStr" r="D19">
+      <c s="24" t="str" r="A19"/>
+      <c s="25" t="str" r="B19"/>
+      <c s="25" t="str" r="C19"/>
+      <c s="17" t="inlineStr" r="D19">
         <is>
           <t xml:space="preserve">Daypart 5</t>
         </is>
       </c>
       <c s="4" t="str" r="E19"/>
       <c s="5" t="str" r="F19"/>
-      <c s="19" r="G19">
-        <v>10</v>
+      <c s="18" r="G19">
+        <v>12</v>
       </c>
       <c s="4" t="str" r="H19"/>
       <c s="5" t="str" r="I19"/>
-      <c s="20" r="J19">
+      <c s="19" r="J19">
         <v>28</v>
       </c>
       <c s="5" t="str" r="K19"/>
-      <c s="21" r="L19">
+      <c s="20" r="L19">
         <v>3</v>
       </c>
       <c s="5" t="str" r="M19"/>
-      <c s="22" r="N19">
+      <c s="21" r="N19">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O19"/>
-      <c s="22" r="P19">
+      <c s="21" r="P19">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q19"/>
-      <c s="22" r="R19">
+      <c s="21" r="R19">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S19"/>
-      <c s="22" r="T19">
+      <c s="21" r="T19">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U19"/>
-      <c s="22" r="V19">
+      <c s="21" r="V19">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W19"/>
       <c s="23" r="X19">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c s="5" t="str" r="Y19"/>
-      <c s="22" r="Z19">
-        <v>19</v>
+      <c s="21" r="Z19">
+        <v>32</v>
       </c>
       <c s="5" t="str" r="AA19"/>
-      <c s="21" r="AB19">
-        <v>133</v>
+      <c s="20" r="AB19">
+        <v>137</v>
       </c>
       <c s="5" t="str" r="AC19"/>
-      <c s="21" r="AD19">
-        <v>66</v>
+      <c s="20" r="AD19">
+        <v>68</v>
       </c>
     </row>
     <row r="20" ht="18" customHeight="0">
-      <c s="16" t="inlineStr" r="A20">
+      <c s="15" t="inlineStr" r="A20">
         <is>
           <t xml:space="preserve">357993 Enola</t>
         </is>
       </c>
-      <c s="17" t="str" r="B20"/>
-      <c s="17" t="str" r="C20"/>
-      <c s="18" t="inlineStr" r="D20">
+      <c s="16" t="str" r="B20"/>
+      <c s="16" t="str" r="C20"/>
+      <c s="17" t="inlineStr" r="D20">
         <is>
           <t xml:space="preserve">Daypart 1</t>
         </is>
       </c>
       <c s="4" t="str" r="E20"/>
       <c s="5" t="str" r="F20"/>
-      <c s="19" r="G20">
+      <c s="18" r="G20">
         <v>5</v>
       </c>
       <c s="4" t="str" r="H20"/>
       <c s="5" t="str" r="I20"/>
       <c s="20" r="J20">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c s="5" t="str" r="K20"/>
-      <c s="21" r="L20">
+      <c s="20" r="L20">
         <v>3</v>
       </c>
       <c s="5" t="str" r="M20"/>
-      <c s="22" r="N20">
+      <c s="21" r="N20">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O20"/>
-      <c s="22" r="P20">
+      <c s="21" r="P20">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q20"/>
-      <c s="22" r="R20">
+      <c s="21" r="R20">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S20"/>
-      <c s="22" r="T20">
+      <c s="21" r="T20">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U20"/>
-      <c s="22" r="V20">
+      <c s="21" r="V20">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W20"/>
-      <c s="28" r="X20">
-        <v>83</v>
+      <c s="26" r="X20">
+        <v>53</v>
       </c>
       <c s="5" t="str" r="Y20"/>
-      <c s="22" r="Z20">
-        <v>21</v>
+      <c s="21" r="Z20">
+        <v>8</v>
       </c>
       <c s="5" t="str" r="AA20"/>
-      <c s="21" r="AB20">
-        <v>128</v>
+      <c s="20" r="AB20">
+        <v>80</v>
       </c>
       <c s="5" t="str" r="AC20"/>
-      <c s="21" r="AD20">
-        <v>128</v>
+      <c s="20" r="AD20">
+        <v>80</v>
       </c>
     </row>
     <row r="21" ht="18" customHeight="0">
-      <c s="24" t="str" r="A21"/>
-      <c s="18" t="inlineStr" r="D21">
+      <c s="22" t="str" r="A21"/>
+      <c s="17" t="inlineStr" r="D21">
         <is>
           <t xml:space="preserve">Daypart 2</t>
         </is>
       </c>
       <c s="4" t="str" r="E21"/>
       <c s="5" t="str" r="F21"/>
-      <c s="19" r="G21">
-        <v>319</v>
+      <c s="18" r="G21">
+        <v>267</v>
       </c>
       <c s="4" t="str" r="H21"/>
       <c s="5" t="str" r="I21"/>
       <c s="23" r="J21">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c s="5" t="str" r="K21"/>
       <c s="20" r="L21">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M21"/>
-      <c s="22" r="N21">
+      <c s="21" r="N21">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O21"/>
-      <c s="22" r="P21">
+      <c s="21" r="P21">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q21"/>
-      <c s="22" r="R21">
+      <c s="21" r="R21">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S21"/>
-      <c s="22" r="T21">
+      <c s="21" r="T21">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U21"/>
-      <c s="22" r="V21">
+      <c s="21" r="V21">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W21"/>
-      <c s="23" r="X21">
-        <v>38</v>
+      <c s="27" r="X21">
+        <v>43</v>
       </c>
       <c s="5" t="str" r="Y21"/>
-      <c s="22" r="Z21">
-        <v>73</v>
+      <c s="21" r="Z21">
+        <v>55</v>
       </c>
       <c s="5" t="str" r="AA21"/>
-      <c s="21" r="AB21">
-        <v>141</v>
+      <c s="20" r="AB21">
+        <v>127</v>
       </c>
       <c s="5" t="str" r="AC21"/>
-      <c s="21" r="AD21">
-        <v>141</v>
+      <c s="20" r="AD21">
+        <v>127</v>
       </c>
     </row>
     <row r="22" ht="18" customHeight="0">
-      <c s="24" t="str" r="A22"/>
-      <c s="18" t="inlineStr" r="D22">
+      <c s="22" t="str" r="A22"/>
+      <c s="17" t="inlineStr" r="D22">
         <is>
           <t xml:space="preserve">Daypart 3</t>
         </is>
       </c>
       <c s="4" t="str" r="E22"/>
       <c s="5" t="str" r="F22"/>
-      <c s="19" r="G22">
-        <v>119</v>
+      <c s="18" r="G22">
+        <v>115</v>
       </c>
       <c s="4" t="str" r="H22"/>
       <c s="5" t="str" r="I22"/>
-      <c s="25" r="J22">
-        <v>32</v>
+      <c s="23" r="J22">
+        <v>27</v>
       </c>
       <c s="5" t="str" r="K22"/>
-      <c s="21" r="L22">
-        <v>4</v>
+      <c s="20" r="L22">
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M22"/>
-      <c s="22" r="N22">
+      <c s="21" r="N22">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O22"/>
-      <c s="22" r="P22">
+      <c s="21" r="P22">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q22"/>
-      <c s="22" r="R22">
+      <c s="21" r="R22">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S22"/>
-      <c s="22" r="T22">
+      <c s="21" r="T22">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U22"/>
-      <c s="22" r="V22">
+      <c s="21" r="V22">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W22"/>
-      <c s="28" r="X22">
-        <v>50</v>
+      <c s="26" r="X22">
+        <v>45</v>
       </c>
       <c s="5" t="str" r="Y22"/>
-      <c s="22" r="Z22">
-        <v>31</v>
+      <c s="21" r="Z22">
+        <v>35</v>
       </c>
       <c s="5" t="str" r="AA22"/>
-      <c s="21" r="AB22">
-        <v>114</v>
+      <c s="20" r="AB22">
+        <v>108</v>
       </c>
       <c s="5" t="str" r="AC22"/>
-      <c s="21" r="AD22">
-        <v>114</v>
+      <c s="20" r="AD22">
+        <v>108</v>
       </c>
     </row>
     <row r="23" ht="18" customHeight="0">
-      <c s="24" t="str" r="A23"/>
-      <c s="18" t="inlineStr" r="D23">
+      <c s="22" t="str" r="A23"/>
+      <c s="17" t="inlineStr" r="D23">
         <is>
           <t xml:space="preserve">Daypart 4</t>
         </is>
       </c>
       <c s="4" t="str" r="E23"/>
       <c s="5" t="str" r="F23"/>
-      <c s="19" r="G23">
-        <v>90</v>
+      <c s="18" r="G23">
+        <v>93</v>
       </c>
       <c s="4" t="str" r="H23"/>
       <c s="5" t="str" r="I23"/>
       <c s="23" r="J23">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c s="5" t="str" r="K23"/>
       <c s="20" r="L23">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c s="5" t="str" r="M23"/>
-      <c s="22" r="N23">
+      <c s="21" r="N23">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O23"/>
-      <c s="22" r="P23">
+      <c s="21" r="P23">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q23"/>
-      <c s="22" r="R23">
+      <c s="21" r="R23">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S23"/>
-      <c s="22" r="T23">
+      <c s="21" r="T23">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U23"/>
-      <c s="22" r="V23">
+      <c s="21" r="V23">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W23"/>
-      <c s="28" r="X23">
-        <v>65</v>
+      <c s="26" r="X23">
+        <v>66</v>
       </c>
       <c s="5" t="str" r="Y23"/>
-      <c s="22" r="Z23">
-        <v>51</v>
+      <c s="21" r="Z23">
+        <v>40</v>
       </c>
       <c s="5" t="str" r="AA23"/>
-      <c s="21" r="AB23">
-        <v>144</v>
+      <c s="20" r="AB23">
+        <v>135</v>
       </c>
       <c s="5" t="str" r="AC23"/>
-      <c s="21" r="AD23">
-        <v>144</v>
+      <c s="20" r="AD23">
+        <v>135</v>
       </c>
     </row>
     <row r="24" ht="18" customHeight="0">
-      <c s="26" t="str" r="A24"/>
-      <c s="27" t="str" r="B24"/>
-      <c s="27" t="str" r="C24"/>
-      <c s="18" t="inlineStr" r="D24">
+      <c s="24" t="str" r="A24"/>
+      <c s="25" t="str" r="B24"/>
+      <c s="25" t="str" r="C24"/>
+      <c s="17" t="inlineStr" r="D24">
         <is>
           <t xml:space="preserve">Daypart 5</t>
         </is>
       </c>
       <c s="4" t="str" r="E24"/>
       <c s="5" t="str" r="F24"/>
-      <c s="19" r="G24">
-        <v>21</v>
+      <c s="18" r="G24">
+        <v>17</v>
       </c>
       <c s="4" t="str" r="H24"/>
       <c s="5" t="str" r="I24"/>
-      <c s="25" r="J24">
-        <v>33</v>
+      <c s="27" r="J24">
+        <v>31</v>
       </c>
       <c s="5" t="str" r="K24"/>
-      <c s="21" r="L24">
-        <v>3</v>
+      <c s="20" r="L24">
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M24"/>
-      <c s="22" r="N24">
+      <c s="21" r="N24">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O24"/>
-      <c s="22" r="P24">
+      <c s="21" r="P24">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q24"/>
-      <c s="22" r="R24">
+      <c s="21" r="R24">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S24"/>
-      <c s="22" r="T24">
+      <c s="21" r="T24">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U24"/>
-      <c s="22" r="V24">
+      <c s="21" r="V24">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W24"/>
-      <c s="28" r="X24">
-        <v>84</v>
+      <c s="26" r="X24">
+        <v>75</v>
       </c>
       <c s="5" t="str" r="Y24"/>
-      <c s="22" r="Z24">
-        <v>23</v>
+      <c s="21" r="Z24">
+        <v>16</v>
       </c>
       <c s="5" t="str" r="AA24"/>
-      <c s="21" r="AB24">
-        <v>138</v>
+      <c s="20" r="AB24">
+        <v>120</v>
       </c>
       <c s="5" t="str" r="AC24"/>
-      <c s="21" r="AD24">
-        <v>138</v>
+      <c s="20" r="AD24">
+        <v>120</v>
       </c>
     </row>
     <row r="25" ht="18" customHeight="0">
-      <c s="16" t="inlineStr" r="A25">
+      <c s="15" t="inlineStr" r="A25">
         <is>
           <t xml:space="preserve">358529 Columbia</t>
         </is>
       </c>
-      <c s="17" t="str" r="B25"/>
-      <c s="17" t="str" r="C25"/>
-      <c s="18" t="inlineStr" r="D25">
+      <c s="16" t="str" r="B25"/>
+      <c s="16" t="str" r="C25"/>
+      <c s="17" t="inlineStr" r="D25">
         <is>
           <t xml:space="preserve">Daypart 2</t>
         </is>
       </c>
       <c s="4" t="str" r="E25"/>
       <c s="5" t="str" r="F25"/>
-      <c s="19" r="G25">
-        <v>246</v>
+      <c s="18" r="G25">
+        <v>248</v>
       </c>
       <c s="4" t="str" r="H25"/>
       <c s="5" t="str" r="I25"/>
-      <c s="25" r="J25">
-        <v>32</v>
+      <c s="23" r="J25">
+        <v>26</v>
       </c>
       <c s="5" t="str" r="K25"/>
-      <c s="23" r="L25">
-        <v>7</v>
+      <c s="20" r="L25">
+        <v>3</v>
       </c>
       <c s="5" t="str" r="M25"/>
-      <c s="22" r="N25">
+      <c s="21" r="N25">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O25"/>
-      <c s="22" r="P25">
+      <c s="21" r="P25">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q25"/>
-      <c s="22" r="R25">
+      <c s="21" r="R25">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S25"/>
-      <c s="22" r="T25">
+      <c s="21" r="T25">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U25"/>
-      <c s="22" r="V25">
+      <c s="21" r="V25">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W25"/>
-      <c s="28" r="X25">
-        <v>49</v>
+      <c s="26" r="X25">
+        <v>48</v>
       </c>
       <c s="5" t="str" r="Y25"/>
-      <c s="22" r="Z25">
-        <v>80</v>
+      <c s="21" r="Z25">
+        <v>70</v>
       </c>
       <c s="5" t="str" r="AA25"/>
       <c s="20" r="AB25">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c s="5" t="str" r="AC25"/>
       <c s="20" r="AD25">
-        <v>161</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" ht="18" customHeight="0">
-      <c s="24" t="str" r="A26"/>
-      <c s="18" t="inlineStr" r="D26">
+      <c s="22" t="str" r="A26"/>
+      <c s="17" t="inlineStr" r="D26">
         <is>
           <t xml:space="preserve">Daypart 3</t>
         </is>
       </c>
       <c s="4" t="str" r="E26"/>
       <c s="5" t="str" r="F26"/>
-      <c s="19" r="G26">
-        <v>88</v>
+      <c s="18" r="G26">
+        <v>99</v>
       </c>
       <c s="4" t="str" r="H26"/>
       <c s="5" t="str" r="I26"/>
-      <c s="28" r="J26">
-        <v>45</v>
+      <c s="26" r="J26">
+        <v>37</v>
       </c>
       <c s="5" t="str" r="K26"/>
       <c s="23" r="L26">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c s="5" t="str" r="M26"/>
-      <c s="22" r="N26">
+      <c s="21" r="N26">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O26"/>
-      <c s="22" r="P26">
+      <c s="21" r="P26">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q26"/>
-      <c s="22" r="R26">
+      <c s="21" r="R26">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S26"/>
-      <c s="22" r="T26">
+      <c s="21" r="T26">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U26"/>
-      <c s="22" r="V26">
+      <c s="21" r="V26">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W26"/>
-      <c s="28" r="X26">
-        <v>65</v>
+      <c s="26" r="X26">
+        <v>74</v>
       </c>
       <c s="5" t="str" r="Y26"/>
-      <c s="22" r="Z26">
-        <v>44</v>
+      <c s="21" r="Z26">
+        <v>45</v>
       </c>
       <c s="5" t="str" r="AA26"/>
-      <c s="20" r="AB26">
-        <v>154</v>
+      <c s="19" r="AB26">
+        <v>156</v>
       </c>
       <c s="5" t="str" r="AC26"/>
-      <c s="20" r="AD26">
-        <v>154</v>
+      <c s="19" r="AD26">
+        <v>156</v>
       </c>
     </row>
     <row r="27" ht="18" customHeight="0">
-      <c s="24" t="str" r="A27"/>
-      <c s="18" t="inlineStr" r="D27">
+      <c s="22" t="str" r="A27"/>
+      <c s="17" t="inlineStr" r="D27">
         <is>
           <t xml:space="preserve">Daypart 4</t>
         </is>
       </c>
       <c s="4" t="str" r="E27"/>
       <c s="5" t="str" r="F27"/>
-      <c s="19" r="G27">
-        <v>71</v>
+      <c s="18" r="G27">
+        <v>75</v>
       </c>
       <c s="4" t="str" r="H27"/>
       <c s="5" t="str" r="I27"/>
-      <c s="28" r="J27">
-        <v>49</v>
+      <c s="26" r="J27">
+        <v>59</v>
       </c>
       <c s="5" t="str" r="K27"/>
-      <c s="20" r="L27">
-        <v>6</v>
+      <c s="26" r="L27">
+        <v>12</v>
       </c>
       <c s="5" t="str" r="M27"/>
-      <c s="22" r="N27">
+      <c s="21" r="N27">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O27"/>
-      <c s="22" r="P27">
+      <c s="21" r="P27">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q27"/>
-      <c s="22" r="R27">
+      <c s="21" r="R27">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S27"/>
-      <c s="22" r="T27">
+      <c s="21" r="T27">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U27"/>
-      <c s="22" r="V27">
+      <c s="21" r="V27">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W27"/>
-      <c s="28" r="X27">
-        <v>84</v>
+      <c s="26" r="X27">
+        <v>88</v>
       </c>
       <c s="5" t="str" r="Y27"/>
-      <c s="22" r="Z27">
-        <v>52</v>
+      <c s="21" r="Z27">
+        <v>34</v>
       </c>
       <c s="5" t="str" r="AA27"/>
-      <c s="25" r="AB27">
-        <v>185</v>
+      <c s="27" r="AB27">
+        <v>181</v>
       </c>
       <c s="5" t="str" r="AC27"/>
-      <c s="25" r="AD27">
-        <v>185</v>
+      <c s="27" r="AD27">
+        <v>181</v>
       </c>
     </row>
     <row r="28" ht="18" customHeight="0">
-      <c s="26" t="str" r="A28"/>
-      <c s="27" t="str" r="B28"/>
-      <c s="27" t="str" r="C28"/>
-      <c s="18" t="inlineStr" r="D28">
+      <c s="24" t="str" r="A28"/>
+      <c s="25" t="str" r="B28"/>
+      <c s="25" t="str" r="C28"/>
+      <c s="17" t="inlineStr" r="D28">
         <is>
           <t xml:space="preserve">Daypart 5</t>
         </is>
       </c>
       <c s="4" t="str" r="E28"/>
       <c s="5" t="str" r="F28"/>
-      <c s="19" r="G28">
-        <v>11</v>
+      <c s="18" r="G28">
+        <v>19</v>
       </c>
       <c s="4" t="str" r="H28"/>
       <c s="5" t="str" r="I28"/>
-      <c s="28" r="J28">
-        <v>38</v>
+      <c s="26" r="J28">
+        <v>51</v>
       </c>
       <c s="5" t="str" r="K28"/>
       <c s="20" r="L28">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M28"/>
-      <c s="22" r="N28">
+      <c s="21" r="N28">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O28"/>
-      <c s="22" r="P28">
+      <c s="21" r="P28">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q28"/>
-      <c s="22" r="R28">
+      <c s="21" r="R28">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S28"/>
-      <c s="22" r="T28">
+      <c s="21" r="T28">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U28"/>
-      <c s="22" r="V28">
+      <c s="21" r="V28">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W28"/>
-      <c s="28" r="X28">
-        <v>107</v>
+      <c s="26" r="X28">
+        <v>115</v>
       </c>
       <c s="5" t="str" r="Y28"/>
-      <c s="22" r="Z28">
-        <v>31</v>
+      <c s="21" r="Z28">
+        <v>26</v>
       </c>
       <c s="5" t="str" r="AA28"/>
-      <c s="23" r="AB28">
-        <v>173</v>
+      <c s="27" r="AB28">
+        <v>193</v>
       </c>
       <c s="5" t="str" r="AC28"/>
-      <c s="23" r="AD28">
-        <v>173</v>
+      <c s="27" r="AD28">
+        <v>193</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="0">
-      <c s="16" t="inlineStr" r="A29">
+      <c s="15" t="inlineStr" r="A29">
         <is>
           <t xml:space="preserve">359042 Lititz</t>
         </is>
       </c>
-      <c s="17" t="str" r="B29"/>
-      <c s="17" t="str" r="C29"/>
-      <c s="18" t="inlineStr" r="D29">
+      <c s="16" t="str" r="B29"/>
+      <c s="16" t="str" r="C29"/>
+      <c s="17" t="inlineStr" r="D29">
         <is>
           <t xml:space="preserve">Daypart 2</t>
         </is>
       </c>
       <c s="4" t="str" r="E29"/>
       <c s="5" t="str" r="F29"/>
-      <c s="19" r="G29">
-        <v>230</v>
+      <c s="18" r="G29">
+        <v>210</v>
       </c>
       <c s="4" t="str" r="H29"/>
       <c s="5" t="str" r="I29"/>
-      <c s="25" r="J29">
-        <v>31</v>
+      <c s="27" r="J29">
+        <v>30</v>
       </c>
       <c s="5" t="str" r="K29"/>
-      <c s="21" r="L29">
-        <v>4</v>
+      <c s="19" r="L29">
+        <v>6</v>
       </c>
       <c s="5" t="str" r="M29"/>
-      <c s="22" r="N29">
+      <c s="21" r="N29">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O29"/>
-      <c s="22" r="P29">
+      <c s="21" r="P29">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q29"/>
-      <c s="22" r="R29">
+      <c s="21" r="R29">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S29"/>
-      <c s="22" r="T29">
+      <c s="21" r="T29">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U29"/>
-      <c s="22" r="V29">
+      <c s="21" r="V29">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W29"/>
-      <c s="28" r="X29">
+      <c s="26" r="X29">
         <v>52</v>
       </c>
       <c s="5" t="str" r="Y29"/>
-      <c s="22" r="Z29">
-        <v>100</v>
+      <c s="21" r="Z29">
+        <v>91</v>
       </c>
       <c s="5" t="str" r="AA29"/>
-      <c s="25" r="AB29">
-        <v>183</v>
+      <c s="23" r="AB29">
+        <v>172</v>
       </c>
       <c s="5" t="str" r="AC29"/>
-      <c s="25" r="AD29">
-        <v>183</v>
+      <c s="23" r="AD29">
+        <v>172</v>
       </c>
     </row>
     <row r="30" ht="18" customHeight="0">
-      <c s="24" t="str" r="A30"/>
-      <c s="18" t="inlineStr" r="D30">
+      <c s="22" t="str" r="A30"/>
+      <c s="17" t="inlineStr" r="D30">
         <is>
           <t xml:space="preserve">Daypart 3</t>
         </is>
       </c>
       <c s="4" t="str" r="E30"/>
       <c s="5" t="str" r="F30"/>
-      <c s="19" r="G30">
-        <v>74</v>
+      <c s="18" r="G30">
+        <v>78</v>
       </c>
       <c s="4" t="str" r="H30"/>
       <c s="5" t="str" r="I30"/>
-      <c s="25" r="J30">
-        <v>33</v>
+      <c s="26" r="J30">
+        <v>42</v>
       </c>
       <c s="5" t="str" r="K30"/>
-      <c s="20" r="L30">
-        <v>5</v>
+      <c s="23" r="L30">
+        <v>7</v>
       </c>
       <c s="5" t="str" r="M30"/>
-      <c s="22" r="N30">
+      <c s="21" r="N30">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O30"/>
-      <c s="22" r="P30">
+      <c s="21" r="P30">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q30"/>
-      <c s="22" r="R30">
+      <c s="21" r="R30">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S30"/>
-      <c s="22" r="T30">
+      <c s="21" r="T30">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U30"/>
-      <c s="22" r="V30">
+      <c s="21" r="V30">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W30"/>
-      <c s="28" r="X30">
-        <v>73</v>
+      <c s="26" r="X30">
+        <v>80</v>
       </c>
       <c s="5" t="str" r="Y30"/>
-      <c s="22" r="Z30">
-        <v>39</v>
+      <c s="21" r="Z30">
+        <v>40</v>
       </c>
       <c s="5" t="str" r="AA30"/>
-      <c s="21" r="AB30">
-        <v>145</v>
+      <c s="19" r="AB30">
+        <v>161</v>
       </c>
       <c s="5" t="str" r="AC30"/>
-      <c s="21" r="AD30">
-        <v>145</v>
+      <c s="19" r="AD30">
+        <v>161</v>
       </c>
     </row>
     <row r="31" ht="18" customHeight="0">
-      <c s="24" t="str" r="A31"/>
-      <c s="18" t="inlineStr" r="D31">
+      <c s="22" t="str" r="A31"/>
+      <c s="17" t="inlineStr" r="D31">
         <is>
           <t xml:space="preserve">Daypart 4</t>
         </is>
       </c>
       <c s="4" t="str" r="E31"/>
       <c s="5" t="str" r="F31"/>
-      <c s="19" r="G31">
-        <v>54</v>
+      <c s="18" r="G31">
+        <v>45</v>
       </c>
       <c s="4" t="str" r="H31"/>
       <c s="5" t="str" r="I31"/>
-      <c s="28" r="J31">
-        <v>66</v>
+      <c s="26" r="J31">
+        <v>58</v>
       </c>
       <c s="5" t="str" r="K31"/>
       <c s="23" r="L31">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c s="5" t="str" r="M31"/>
-      <c s="22" r="N31">
+      <c s="21" r="N31">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O31"/>
-      <c s="22" r="P31">
+      <c s="21" r="P31">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q31"/>
-      <c s="22" r="R31">
+      <c s="21" r="R31">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S31"/>
-      <c s="22" r="T31">
+      <c s="21" r="T31">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U31"/>
-      <c s="22" r="V31">
+      <c s="21" r="V31">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W31"/>
-      <c s="28" r="X31">
-        <v>126</v>
+      <c s="26" r="X31">
+        <v>92</v>
       </c>
       <c s="5" t="str" r="Y31"/>
-      <c s="22" r="Z31">
-        <v>72</v>
+      <c s="21" r="Z31">
+        <v>32</v>
       </c>
       <c s="5" t="str" r="AA31"/>
-      <c s="28" r="AB31">
-        <v>263</v>
+      <c s="27" r="AB31">
+        <v>181</v>
       </c>
       <c s="5" t="str" r="AC31"/>
-      <c s="28" r="AD31">
-        <v>263</v>
+      <c s="27" r="AD31">
+        <v>181</v>
       </c>
     </row>
     <row r="32" ht="18" customHeight="0">
-      <c s="26" t="str" r="A32"/>
-      <c s="27" t="str" r="B32"/>
-      <c s="27" t="str" r="C32"/>
-      <c s="18" t="inlineStr" r="D32">
+      <c s="24" t="str" r="A32"/>
+      <c s="25" t="str" r="B32"/>
+      <c s="25" t="str" r="C32"/>
+      <c s="17" t="inlineStr" r="D32">
         <is>
           <t xml:space="preserve">Daypart 5</t>
         </is>
       </c>
       <c s="4" t="str" r="E32"/>
       <c s="5" t="str" r="F32"/>
-      <c s="19" r="G32">
-        <v>12</v>
+      <c s="18" r="G32">
+        <v>9</v>
       </c>
       <c s="4" t="str" r="H32"/>
       <c s="5" t="str" r="I32"/>
-      <c s="28" r="J32">
-        <v>46</v>
+      <c s="27" r="J32">
+        <v>31</v>
       </c>
       <c s="5" t="str" r="K32"/>
-      <c s="21" r="L32">
-        <v>2</v>
+      <c s="20" r="L32">
+        <v>3</v>
       </c>
       <c s="5" t="str" r="M32"/>
-      <c s="22" r="N32">
+      <c s="21" r="N32">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O32"/>
-      <c s="22" r="P32">
+      <c s="21" r="P32">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q32"/>
-      <c s="22" r="R32">
+      <c s="21" r="R32">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S32"/>
-      <c s="22" r="T32">
+      <c s="21" r="T32">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U32"/>
-      <c s="22" r="V32">
+      <c s="21" r="V32">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W32"/>
-      <c s="28" r="X32">
-        <v>159</v>
+      <c s="26" r="X32">
+        <v>90</v>
       </c>
       <c s="5" t="str" r="Y32"/>
-      <c s="22" r="Z32">
-        <v>14</v>
+      <c s="21" r="Z32">
+        <v>18</v>
       </c>
       <c s="5" t="str" r="AA32"/>
-      <c s="28" r="AB32">
-        <v>220</v>
+      <c s="20" r="AB32">
+        <v>140</v>
       </c>
       <c s="5" t="str" r="AC32"/>
-      <c s="28" r="AD32">
-        <v>220</v>
+      <c s="20" r="AD32">
+        <v>140</v>
       </c>
     </row>
     <row r="33" ht="18" customHeight="0">
-      <c s="16" t="inlineStr" r="A33">
+      <c s="15" t="inlineStr" r="A33">
         <is>
           <t xml:space="preserve">362913 Eisenhower</t>
         </is>
       </c>
-      <c s="17" t="str" r="B33"/>
-      <c s="17" t="str" r="C33"/>
-      <c s="18" t="inlineStr" r="D33">
+      <c s="16" t="str" r="B33"/>
+      <c s="16" t="str" r="C33"/>
+      <c s="17" t="inlineStr" r="D33">
         <is>
           <t xml:space="preserve">Daypart 2</t>
         </is>
       </c>
       <c s="4" t="str" r="E33"/>
       <c s="5" t="str" r="F33"/>
-      <c s="19" r="G33">
-        <v>169</v>
+      <c s="18" r="G33">
+        <v>167</v>
       </c>
       <c s="4" t="str" r="H33"/>
       <c s="5" t="str" r="I33"/>
-      <c s="20" r="J33">
-        <v>31</v>
+      <c s="19" r="J33">
+        <v>33</v>
       </c>
       <c s="5" t="str" r="K33"/>
-      <c s="21" r="L33">
-        <v>2</v>
+      <c s="20" r="L33">
+        <v>3</v>
       </c>
       <c s="5" t="str" r="M33"/>
-      <c s="22" r="N33">
+      <c s="21" r="N33">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O33"/>
-      <c s="22" r="P33">
+      <c s="21" r="P33">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q33"/>
-      <c s="22" r="R33">
+      <c s="21" r="R33">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S33"/>
-      <c s="22" r="T33">
+      <c s="21" r="T33">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U33"/>
       <c s="20" r="V33">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c s="5" t="str" r="W33"/>
-      <c s="28" r="X33">
-        <v>48</v>
+      <c s="26" r="X33">
+        <v>51</v>
       </c>
       <c s="5" t="str" r="Y33"/>
-      <c s="22" r="Z33">
+      <c s="21" r="Z33">
         <v>40</v>
       </c>
       <c s="5" t="str" r="AA33"/>
-      <c s="21" r="AB33">
+      <c s="20" r="AB33">
         <v>95</v>
       </c>
       <c s="5" t="str" r="AC33"/>
-      <c s="20" r="AD33">
+      <c s="19" r="AD33">
         <v>136</v>
       </c>
     </row>
     <row r="34" ht="18" customHeight="0">
-      <c s="24" t="str" r="A34"/>
-      <c s="18" t="inlineStr" r="D34">
+      <c s="22" t="str" r="A34"/>
+      <c s="17" t="inlineStr" r="D34">
         <is>
           <t xml:space="preserve">Daypart 3</t>
         </is>
       </c>
       <c s="4" t="str" r="E34"/>
       <c s="5" t="str" r="F34"/>
-      <c s="19" r="G34">
-        <v>58</v>
+      <c s="18" r="G34">
+        <v>50</v>
       </c>
       <c s="4" t="str" r="H34"/>
       <c s="5" t="str" r="I34"/>
-      <c s="20" r="J34">
-        <v>39</v>
+      <c s="19" r="J34">
+        <v>37</v>
       </c>
       <c s="5" t="str" r="K34"/>
-      <c s="21" r="L34">
-        <v>2</v>
+      <c s="20" r="L34">
+        <v>3</v>
       </c>
       <c s="5" t="str" r="M34"/>
-      <c s="22" r="N34">
+      <c s="21" r="N34">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O34"/>
-      <c s="22" r="P34">
+      <c s="21" r="P34">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q34"/>
-      <c s="22" r="R34">
+      <c s="21" r="R34">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S34"/>
-      <c s="22" r="T34">
+      <c s="21" r="T34">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U34"/>
-      <c s="21" r="V34">
-        <v>5</v>
+      <c s="20" r="V34">
+        <v>6</v>
       </c>
       <c s="5" t="str" r="W34"/>
-      <c s="28" r="X34">
-        <v>53</v>
+      <c s="26" r="X34">
+        <v>88</v>
       </c>
       <c s="5" t="str" r="Y34"/>
-      <c s="22" r="Z34">
-        <v>19</v>
+      <c s="21" r="Z34">
+        <v>28</v>
       </c>
       <c s="5" t="str" r="AA34"/>
-      <c s="21" r="AB34">
-        <v>95</v>
+      <c s="19" r="AB34">
+        <v>129</v>
       </c>
       <c s="5" t="str" r="AC34"/>
-      <c s="21" r="AD34">
-        <v>115</v>
+      <c s="19" r="AD34">
+        <v>158</v>
       </c>
     </row>
     <row r="35" ht="18" customHeight="0">
-      <c s="24" t="str" r="A35"/>
-      <c s="18" t="inlineStr" r="D35">
+      <c s="22" t="str" r="A35"/>
+      <c s="17" t="inlineStr" r="D35">
         <is>
           <t xml:space="preserve">Daypart 4</t>
         </is>
       </c>
       <c s="4" t="str" r="E35"/>
       <c s="5" t="str" r="F35"/>
-      <c s="19" r="G35">
-        <v>42</v>
+      <c s="18" r="G35">
+        <v>39</v>
       </c>
       <c s="4" t="str" r="H35"/>
       <c s="5" t="str" r="I35"/>
-      <c s="20" r="J35">
-        <v>39</v>
+      <c s="23" r="J35">
+        <v>48</v>
       </c>
       <c s="5" t="str" r="K35"/>
-      <c s="21" r="L35">
-        <v>3</v>
+      <c s="19" r="L35">
+        <v>5</v>
       </c>
       <c s="5" t="str" r="M35"/>
-      <c s="22" r="N35">
+      <c s="21" r="N35">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O35"/>
-      <c s="22" r="P35">
+      <c s="21" r="P35">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q35"/>
-      <c s="22" r="R35">
+      <c s="21" r="R35">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S35"/>
-      <c s="22" r="T35">
+      <c s="21" r="T35">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U35"/>
-      <c s="21" r="V35">
-        <v>4</v>
+      <c s="20" r="V35">
+        <v>13</v>
       </c>
       <c s="5" t="str" r="W35"/>
-      <c s="28" r="X35">
-        <v>104</v>
+      <c s="26" r="X35">
+        <v>126</v>
       </c>
       <c s="5" t="str" r="Y35"/>
-      <c s="22" r="Z35">
-        <v>32</v>
+      <c s="21" r="Z35">
+        <v>36</v>
       </c>
       <c s="5" t="str" r="AA35"/>
-      <c s="20" r="AB35">
-        <v>146</v>
+      <c s="23" r="AB35">
+        <v>183</v>
       </c>
       <c s="5" t="str" r="AC35"/>
-      <c s="20" r="AD35">
-        <v>178</v>
+      <c s="23" r="AD35">
+        <v>220</v>
       </c>
     </row>
     <row r="36" ht="18" customHeight="0">
-      <c s="26" t="str" r="A36"/>
-      <c s="27" t="str" r="B36"/>
-      <c s="27" t="str" r="C36"/>
-      <c s="18" t="inlineStr" r="D36">
+      <c s="24" t="str" r="A36"/>
+      <c s="25" t="str" r="B36"/>
+      <c s="25" t="str" r="C36"/>
+      <c s="17" t="inlineStr" r="D36">
         <is>
           <t xml:space="preserve">Daypart 5</t>
         </is>
       </c>
       <c s="4" t="str" r="E36"/>
       <c s="5" t="str" r="F36"/>
-      <c s="19" r="G36">
+      <c s="18" r="G36">
         <v>8</v>
       </c>
       <c s="4" t="str" r="H36"/>
       <c s="5" t="str" r="I36"/>
-      <c s="23" r="J36">
-        <v>49</v>
+      <c s="26" r="J36">
+        <v>61</v>
       </c>
       <c s="5" t="str" r="K36"/>
-      <c s="21" r="L36">
-        <v>3</v>
+      <c s="19" r="L36">
+        <v>6</v>
       </c>
       <c s="5" t="str" r="M36"/>
-      <c s="22" r="N36">
+      <c s="21" r="N36">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O36"/>
-      <c s="22" r="P36">
+      <c s="21" r="P36">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q36"/>
-      <c s="22" r="R36">
+      <c s="21" r="R36">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S36"/>
-      <c s="22" r="T36">
+      <c s="21" r="T36">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U36"/>
-      <c s="23" r="V36">
-        <v>23</v>
+      <c s="20" r="V36">
+        <v>10</v>
       </c>
       <c s="5" t="str" r="W36"/>
-      <c s="28" r="X36">
-        <v>78</v>
+      <c s="26" r="X36">
+        <v>210</v>
       </c>
       <c s="5" t="str" r="Y36"/>
-      <c s="22" r="Z36">
-        <v>9</v>
+      <c s="21" r="Z36">
+        <v>11</v>
       </c>
       <c s="5" t="str" r="AA36"/>
-      <c s="20" r="AB36">
-        <v>134</v>
+      <c s="27" r="AB36">
+        <v>273</v>
       </c>
       <c s="5" t="str" r="AC36"/>
-      <c s="20" r="AD36">
-        <v>144</v>
+      <c s="27" r="AD36">
+        <v>284</v>
       </c>
     </row>
     <row r="37" ht="18" customHeight="0">
-      <c s="16" t="inlineStr" r="A37">
+      <c s="15" t="inlineStr" r="A37">
         <is>
           <t xml:space="preserve">363271 Marietta</t>
         </is>
       </c>
-      <c s="17" t="str" r="B37"/>
-      <c s="17" t="str" r="C37"/>
-      <c s="18" t="inlineStr" r="D37">
+      <c s="16" t="str" r="B37"/>
+      <c s="16" t="str" r="C37"/>
+      <c s="17" t="inlineStr" r="D37">
         <is>
           <t xml:space="preserve">Daypart 2</t>
         </is>
       </c>
       <c s="4" t="str" r="E37"/>
       <c s="5" t="str" r="F37"/>
-      <c s="19" r="G37">
-        <v>248</v>
+      <c s="18" r="G37">
+        <v>225</v>
       </c>
       <c s="4" t="str" r="H37"/>
       <c s="5" t="str" r="I37"/>
-      <c s="22" r="J37">
+      <c s="21" r="J37">
         <v>0</v>
       </c>
       <c s="5" t="str" r="K37"/>
-      <c s="22" r="L37">
+      <c s="21" r="L37">
         <v>0</v>
       </c>
       <c s="5" t="str" r="M37"/>
       <c s="23" r="N37">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c s="5" t="str" r="O37"/>
-      <c s="21" r="P37">
-        <v>3</v>
+      <c s="20" r="P37">
+        <v>2</v>
       </c>
       <c s="5" t="str" r="Q37"/>
-      <c s="21" r="R37">
+      <c s="20" r="R37">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S37"/>
-      <c s="21" r="T37">
-        <v>1</v>
+      <c s="20" r="T37">
+        <v>0</v>
       </c>
       <c s="5" t="str" r="U37"/>
-      <c s="22" r="V37">
+      <c s="21" r="V37">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W37"/>
-      <c s="28" r="X37">
+      <c s="26" r="X37">
         <v>48</v>
       </c>
       <c s="5" t="str" r="Y37"/>
-      <c s="22" r="Z37">
-        <v>68</v>
+      <c s="21" r="Z37">
+        <v>50</v>
       </c>
       <c s="5" t="str" r="AA37"/>
-      <c s="21" r="AB37">
-        <v>142</v>
+      <c s="20" r="AB37">
+        <v>123</v>
       </c>
       <c s="5" t="str" r="AC37"/>
-      <c s="21" r="AD37">
-        <v>142</v>
+      <c s="20" r="AD37">
+        <v>123</v>
       </c>
     </row>
     <row r="38" ht="18" customHeight="0">
-      <c s="24" t="str" r="A38"/>
-      <c s="18" t="inlineStr" r="D38">
+      <c s="22" t="str" r="A38"/>
+      <c s="17" t="inlineStr" r="D38">
         <is>
           <t xml:space="preserve">Daypart 3</t>
         </is>
       </c>
       <c s="4" t="str" r="E38"/>
       <c s="5" t="str" r="F38"/>
-      <c s="19" r="G38">
-        <v>80</v>
+      <c s="18" r="G38">
+        <v>71</v>
       </c>
       <c s="4" t="str" r="H38"/>
       <c s="5" t="str" r="I38"/>
-      <c s="22" r="J38">
+      <c s="21" r="J38">
         <v>0</v>
       </c>
       <c s="5" t="str" r="K38"/>
-      <c s="22" r="L38">
+      <c s="21" r="L38">
         <v>0</v>
       </c>
       <c s="5" t="str" r="M38"/>
-      <c s="28" r="N38">
-        <v>37</v>
+      <c s="27" r="N38">
+        <v>34</v>
       </c>
       <c s="5" t="str" r="O38"/>
-      <c s="21" r="P38">
-        <v>4</v>
+      <c s="20" r="P38">
+        <v>3</v>
       </c>
       <c s="5" t="str" r="Q38"/>
-      <c s="21" r="R38">
+      <c s="20" r="R38">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S38"/>
-      <c s="21" r="T38">
+      <c s="20" r="T38">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U38"/>
-      <c s="22" r="V38">
+      <c s="21" r="V38">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W38"/>
-      <c s="28" r="X38">
-        <v>90</v>
+      <c s="26" r="X38">
+        <v>97</v>
       </c>
       <c s="5" t="str" r="Y38"/>
-      <c s="22" r="Z38">
-        <v>46</v>
+      <c s="21" r="Z38">
+        <v>98</v>
       </c>
       <c s="5" t="str" r="AA38"/>
-      <c s="23" r="AB38">
-        <v>174</v>
+      <c s="26" r="AB38">
+        <v>230</v>
       </c>
       <c s="5" t="str" r="AC38"/>
-      <c s="23" r="AD38">
-        <v>174</v>
+      <c s="26" r="AD38">
+        <v>230</v>
       </c>
     </row>
     <row r="39" ht="18" customHeight="0">
-      <c s="24" t="str" r="A39"/>
-      <c s="18" t="inlineStr" r="D39">
+      <c s="22" t="str" r="A39"/>
+      <c s="17" t="inlineStr" r="D39">
         <is>
           <t xml:space="preserve">Daypart 4</t>
         </is>
       </c>
       <c s="4" t="str" r="E39"/>
       <c s="5" t="str" r="F39"/>
-      <c s="19" r="G39">
-        <v>58</v>
+      <c s="18" r="G39">
+        <v>55</v>
       </c>
       <c s="4" t="str" r="H39"/>
       <c s="5" t="str" r="I39"/>
-      <c s="22" r="J39">
+      <c s="21" r="J39">
         <v>0</v>
       </c>
       <c s="5" t="str" r="K39"/>
-      <c s="22" r="L39">
+      <c s="21" r="L39">
         <v>0</v>
       </c>
       <c s="5" t="str" r="M39"/>
-      <c s="25" r="N39">
-        <v>31</v>
+      <c s="26" r="N39">
+        <v>36</v>
       </c>
       <c s="5" t="str" r="O39"/>
-      <c s="21" r="P39">
+      <c s="20" r="P39">
         <v>3</v>
       </c>
       <c s="5" t="str" r="Q39"/>
-      <c s="22" r="R39">
+      <c s="21" r="R39">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S39"/>
-      <c s="22" r="T39">
+      <c s="21" r="T39">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U39"/>
-      <c s="22" r="V39">
+      <c s="21" r="V39">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W39"/>
-      <c s="28" r="X39">
-        <v>65</v>
+      <c s="26" r="X39">
+        <v>75</v>
       </c>
       <c s="5" t="str" r="Y39"/>
-      <c s="22" r="Z39">
+      <c s="21" r="Z39">
         <v>28</v>
       </c>
       <c s="5" t="str" r="AA39"/>
-      <c s="21" r="AB39">
-        <v>125</v>
+      <c s="20" r="AB39">
+        <v>141</v>
       </c>
       <c s="5" t="str" r="AC39"/>
-      <c s="21" r="AD39">
-        <v>125</v>
+      <c s="20" r="AD39">
+        <v>141</v>
       </c>
     </row>
     <row r="40" ht="18" customHeight="0">
-      <c s="26" t="str" r="A40"/>
-      <c s="27" t="str" r="B40"/>
-      <c s="27" t="str" r="C40"/>
-      <c s="18" t="inlineStr" r="D40">
+      <c s="24" t="str" r="A40"/>
+      <c s="25" t="str" r="B40"/>
+      <c s="25" t="str" r="C40"/>
+      <c s="17" t="inlineStr" r="D40">
         <is>
           <t xml:space="preserve">Daypart 5</t>
         </is>
       </c>
       <c s="4" t="str" r="E40"/>
       <c s="5" t="str" r="F40"/>
-      <c s="19" r="G40">
-        <v>14</v>
+      <c s="18" r="G40">
+        <v>12</v>
       </c>
       <c s="4" t="str" r="H40"/>
       <c s="5" t="str" r="I40"/>
-      <c s="22" r="J40">
+      <c s="21" r="J40">
         <v>0</v>
       </c>
       <c s="5" t="str" r="K40"/>
-      <c s="22" r="L40">
+      <c s="21" r="L40">
         <v>0</v>
       </c>
       <c s="5" t="str" r="M40"/>
-      <c s="25" r="N40">
-        <v>32</v>
+      <c s="23" r="N40">
+        <v>27</v>
       </c>
       <c s="5" t="str" r="O40"/>
-      <c s="21" r="P40">
+      <c s="20" r="P40">
         <v>2</v>
       </c>
       <c s="5" t="str" r="Q40"/>
-      <c s="22" r="R40">
+      <c s="21" r="R40">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S40"/>
-      <c s="22" r="T40">
+      <c s="21" r="T40">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U40"/>
-      <c s="22" r="V40">
+      <c s="21" r="V40">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W40"/>
-      <c s="28" r="X40">
-        <v>87</v>
+      <c s="26" r="X40">
+        <v>68</v>
       </c>
       <c s="5" t="str" r="Y40"/>
-      <c s="22" r="Z40">
-        <v>10</v>
+      <c s="21" r="Z40">
+        <v>9</v>
       </c>
       <c s="5" t="str" r="AA40"/>
-      <c s="21" r="AB40">
-        <v>130</v>
+      <c s="20" r="AB40">
+        <v>105</v>
       </c>
       <c s="5" t="str" r="AC40"/>
-      <c s="21" r="AD40">
-        <v>130</v>
+      <c s="20" r="AD40">
+        <v>105</v>
       </c>
     </row>
     <row r="41" ht="18" customHeight="0">
-      <c s="16" t="inlineStr" r="A41">
+      <c s="15" t="inlineStr" r="A41">
         <is>
           <t xml:space="preserve">364322 E-Town</t>
         </is>
       </c>
-      <c s="17" t="str" r="B41"/>
-      <c s="17" t="str" r="C41"/>
-      <c s="18" t="inlineStr" r="D41">
+      <c s="16" t="str" r="B41"/>
+      <c s="16" t="str" r="C41"/>
+      <c s="17" t="inlineStr" r="D41">
         <is>
           <t xml:space="preserve">Daypart 2</t>
         </is>
       </c>
       <c s="4" t="str" r="E41"/>
       <c s="5" t="str" r="F41"/>
-      <c s="19" r="G41">
-        <v>186</v>
+      <c s="18" r="G41">
+        <v>223</v>
       </c>
       <c s="4" t="str" r="H41"/>
       <c s="5" t="str" r="I41"/>
-      <c s="28" r="J41">
-        <v>63</v>
+      <c s="20" r="J41">
+        <v>27</v>
       </c>
       <c s="5" t="str" r="K41"/>
       <c s="20" r="L41">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M41"/>
-      <c s="22" r="N41">
+      <c s="21" r="N41">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O41"/>
-      <c s="22" r="P41">
+      <c s="21" r="P41">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q41"/>
-      <c s="22" r="R41">
+      <c s="21" r="R41">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S41"/>
-      <c s="22" r="T41">
+      <c s="21" r="T41">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U41"/>
-      <c s="23" r="V41">
-        <v>23</v>
+      <c s="19" r="V41">
+        <v>15</v>
       </c>
       <c s="5" t="str" r="W41"/>
-      <c s="28" r="X41">
-        <v>81</v>
+      <c s="26" r="X41">
+        <v>46</v>
       </c>
       <c s="5" t="str" r="Y41"/>
-      <c s="22" r="Z41">
-        <v>93</v>
+      <c s="21" r="Z41">
+        <v>52</v>
       </c>
       <c s="5" t="str" r="AA41"/>
-      <c s="25" r="AB41">
-        <v>254</v>
+      <c s="20" r="AB41">
+        <v>138</v>
       </c>
       <c s="5" t="str" r="AC41"/>
-      <c s="25" r="AD41">
-        <v>254</v>
+      <c s="20" r="AD41">
+        <v>138</v>
       </c>
     </row>
     <row r="42" ht="18" customHeight="0">
-      <c s="24" t="str" r="A42"/>
-      <c s="18" t="inlineStr" r="D42">
+      <c s="22" t="str" r="A42"/>
+      <c s="17" t="inlineStr" r="D42">
         <is>
           <t xml:space="preserve">Daypart 3</t>
         </is>
       </c>
       <c s="4" t="str" r="E42"/>
       <c s="5" t="str" r="F42"/>
-      <c s="19" r="G42">
-        <v>76</v>
+      <c s="18" r="G42">
+        <v>98</v>
       </c>
       <c s="4" t="str" r="H42"/>
       <c s="5" t="str" r="I42"/>
-      <c s="23" r="J42">
-        <v>41</v>
+      <c s="20" r="J42">
+        <v>28</v>
       </c>
       <c s="5" t="str" r="K42"/>
-      <c s="21" r="L42">
-        <v>4</v>
+      <c s="20" r="L42">
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M42"/>
-      <c s="22" r="N42">
+      <c s="21" r="N42">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O42"/>
-      <c s="22" r="P42">
+      <c s="21" r="P42">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q42"/>
-      <c s="22" r="R42">
+      <c s="21" r="R42">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S42"/>
-      <c s="22" r="T42">
+      <c s="21" r="T42">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U42"/>
-      <c s="21" r="V42">
-        <v>3</v>
+      <c s="20" r="V42">
+        <v>10</v>
       </c>
       <c s="5" t="str" r="W42"/>
-      <c s="28" r="X42">
-        <v>74</v>
+      <c s="26" r="X42">
+        <v>58</v>
       </c>
       <c s="5" t="str" r="Y42"/>
-      <c s="22" r="Z42">
-        <v>30</v>
+      <c s="21" r="Z42">
+        <v>34</v>
       </c>
       <c s="5" t="str" r="AA42"/>
-      <c s="21" r="AB42">
-        <v>146</v>
+      <c s="20" r="AB42">
+        <v>128</v>
       </c>
       <c s="5" t="str" r="AC42"/>
-      <c s="21" r="AD42">
-        <v>146</v>
+      <c s="20" r="AD42">
+        <v>128</v>
       </c>
     </row>
     <row r="43" ht="18" customHeight="0">
-      <c s="24" t="str" r="A43"/>
-      <c s="18" t="inlineStr" r="D43">
+      <c s="22" t="str" r="A43"/>
+      <c s="17" t="inlineStr" r="D43">
         <is>
           <t xml:space="preserve">Daypart 4</t>
         </is>
       </c>
       <c s="4" t="str" r="E43"/>
       <c s="5" t="str" r="F43"/>
-      <c s="19" r="G43">
-        <v>72</v>
+      <c s="18" r="G43">
+        <v>75</v>
       </c>
       <c s="4" t="str" r="H43"/>
       <c s="5" t="str" r="I43"/>
       <c s="23" r="J43">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c s="5" t="str" r="K43"/>
       <c s="20" r="L43">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c s="5" t="str" r="M43"/>
-      <c s="22" r="N43">
+      <c s="21" r="N43">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O43"/>
-      <c s="22" r="P43">
+      <c s="21" r="P43">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q43"/>
-      <c s="22" r="R43">
+      <c s="21" r="R43">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S43"/>
-      <c s="22" r="T43">
+      <c s="21" r="T43">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U43"/>
-      <c s="21" r="V43">
-        <v>11</v>
+      <c s="19" r="V43">
+        <v>17</v>
       </c>
       <c s="5" t="str" r="W43"/>
-      <c s="28" r="X43">
-        <v>92</v>
+      <c s="26" r="X43">
+        <v>97</v>
       </c>
       <c s="5" t="str" r="Y43"/>
-      <c s="22" r="Z43">
-        <v>33</v>
+      <c s="21" r="Z43">
+        <v>56</v>
       </c>
       <c s="5" t="str" r="AA43"/>
-      <c s="20" r="AB43">
-        <v>173</v>
+      <c s="23" r="AB43">
+        <v>205</v>
       </c>
       <c s="5" t="str" r="AC43"/>
-      <c s="20" r="AD43">
-        <v>173</v>
+      <c s="23" r="AD43">
+        <v>205</v>
       </c>
     </row>
     <row r="44" ht="18" customHeight="0">
-      <c s="26" t="str" r="A44"/>
-      <c s="27" t="str" r="B44"/>
-      <c s="27" t="str" r="C44"/>
-      <c s="18" t="inlineStr" r="D44">
+      <c s="24" t="str" r="A44"/>
+      <c s="25" t="str" r="B44"/>
+      <c s="25" t="str" r="C44"/>
+      <c s="17" t="inlineStr" r="D44">
         <is>
           <t xml:space="preserve">Daypart 5</t>
         </is>
       </c>
       <c s="4" t="str" r="E44"/>
       <c s="5" t="str" r="F44"/>
-      <c s="19" r="G44">
+      <c s="18" r="G44">
         <v>14</v>
       </c>
       <c s="4" t="str" r="H44"/>
       <c s="5" t="str" r="I44"/>
       <c s="20" r="J44">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c s="5" t="str" r="K44"/>
       <c s="20" r="L44">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c s="5" t="str" r="M44"/>
-      <c s="22" r="N44">
+      <c s="21" r="N44">
         <v>0</v>
       </c>
       <c s="5" t="str" r="O44"/>
-      <c s="22" r="P44">
+      <c s="21" r="P44">
         <v>0</v>
       </c>
       <c s="5" t="str" r="Q44"/>
-      <c s="22" r="R44">
+      <c s="21" r="R44">
         <v>0</v>
       </c>
       <c s="5" t="str" r="S44"/>
-      <c s="22" r="T44">
+      <c s="21" r="T44">
         <v>0</v>
       </c>
       <c s="5" t="str" r="U44"/>
-      <c s="21" r="V44">
-        <v>2</v>
+      <c s="20" r="V44">
+        <v>1</v>
       </c>
       <c s="5" t="str" r="W44"/>
-      <c s="28" r="X44">
+      <c s="26" r="X44">
         <v>107</v>
       </c>
       <c s="5" t="str" r="Y44"/>
-      <c s="22" r="Z44">
-        <v>15</v>
+      <c s="21" r="Z44">
+        <v>20</v>
       </c>
       <c s="5" t="str" r="AA44"/>
-      <c s="21" r="AB44">
-        <v>148</v>
+      <c s="19" r="AB44">
+        <v>151</v>
       </c>
       <c s="5" t="str" r="AC44"/>
-      <c s="21" r="AD44">
-        <v>148</v>
+      <c s="19" r="AD44">
+        <v>151</v>
       </c>
     </row>
     <row r="45" ht="0.05" customHeight="1"/>
@@ -3291,7 +3288,7 @@
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.95" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;L&amp;"Segoe UI,Italic"&amp;9 Print Date &amp;&amp; Time: 2/5/2026 12:44:12 PM 
+    <oddFooter>&amp;L&amp;"Segoe UI,Italic"&amp;9 Print Date &amp;&amp; Time: 2/6/2026 12:45:23 PM 
 &amp;"-,Italic"Page Number:  &amp;P </oddFooter>
   </headerFooter>
   <drawing r:id="rId7"/>

</xml_diff>

<commit_message>
update on sorting and table
</commit_message>
<xml_diff>
--- a/data/hme/raw/hme_report.xlsx
+++ b/data/hme/raw/hme_report.xlsx
@@ -146,12 +146,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE35454"/>
-        <bgColor rgb="FFE35454"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFB40000"/>
         <bgColor rgb="FFB40000"/>
       </patternFill>
@@ -160,6 +154,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF540202"/>
         <bgColor rgb="FF540202"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE35454"/>
+        <bgColor rgb="FFE35454"/>
       </patternFill>
     </fill>
   </fills>
@@ -336,10 +336,7 @@
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="0" fontId="1" fillId="3" borderId="6">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="6" borderId="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="7" borderId="1">
+    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="8" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="0" fontId="1" fillId="3" borderId="7">
@@ -348,7 +345,10 @@
     <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="0" fontId="1" fillId="0" borderId="8">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="8" borderId="1">
+    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="7" borderId="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" numFmtId="83" fontId="9" fillId="6" borderId="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -375,9 +375,9 @@
       <rgbColor rgb="00333333"/>
       <rgbColor rgb="00F4D216"/>
       <rgbColor rgb="0000B04C"/>
-      <rgbColor rgb="00E35454"/>
       <rgbColor rgb="00B40000"/>
       <rgbColor rgb="00540202"/>
+      <rgbColor rgb="00E35454"/>
       <rgbColor rgb="00808000"/>
       <rgbColor rgb="00800080"/>
       <rgbColor rgb="00008080"/>
@@ -520,7 +520,7 @@
     <row r="3" ht="18.15" customHeight="1">
       <c s="2" t="inlineStr" r="C3">
         <is>
-          <t xml:space="preserve">Day: 02/07/2026</t>
+          <t xml:space="preserve">Day: 02/08/2026</t>
         </is>
       </c>
     </row>
@@ -616,10 +616,10 @@
       <c s="4" t="str" r="C7"/>
       <c s="5" t="str" r="D7"/>
       <c s="7" r="E7">
-        <v>331</v>
+        <v>305</v>
       </c>
       <c s="8" r="F7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c s="5" t="str" r="G7"/>
       <c s="9" r="H7">
@@ -645,20 +645,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="R7"/>
-      <c s="11" r="S7">
-        <v>63</v>
+      <c s="8" r="S7">
+        <v>58</v>
       </c>
       <c s="5" t="str" r="T7"/>
       <c s="10" r="U7">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c s="5" t="str" r="V7"/>
       <c s="9" r="W7">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c s="5" t="str" r="X7"/>
       <c s="9" r="Y7">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c s="5" t="str" r="Z7"/>
     </row>
@@ -672,14 +672,14 @@
       <c s="4" t="str" r="C8"/>
       <c s="5" t="str" r="D8"/>
       <c s="7" r="E8">
-        <v>529</v>
-      </c>
-      <c s="12" r="F8">
-        <v>33</v>
+        <v>452</v>
+      </c>
+      <c s="11" r="F8">
+        <v>31</v>
       </c>
       <c s="5" t="str" r="G8"/>
       <c s="9" r="H8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c s="10" r="I8">
         <v>0</v>
@@ -701,20 +701,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="R8"/>
-      <c s="13" r="S8">
-        <v>56</v>
+      <c s="12" r="S8">
+        <v>51</v>
       </c>
       <c s="5" t="str" r="T8"/>
       <c s="10" r="U8">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c s="5" t="str" r="V8"/>
-      <c s="8" r="W8">
-        <v>159</v>
+      <c s="9" r="W8">
+        <v>128</v>
       </c>
       <c s="5" t="str" r="X8"/>
-      <c s="8" r="Y8">
-        <v>159</v>
+      <c s="9" r="Y8">
+        <v>128</v>
       </c>
       <c s="5" t="str" r="Z8"/>
     </row>
@@ -728,14 +728,14 @@
       <c s="4" t="str" r="C9"/>
       <c s="5" t="str" r="D9"/>
       <c s="7" r="E9">
-        <v>390</v>
-      </c>
-      <c s="13" r="F9">
-        <v>46</v>
+        <v>371</v>
+      </c>
+      <c s="12" r="F9">
+        <v>49</v>
       </c>
       <c s="5" t="str" r="G9"/>
       <c s="11" r="H9">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c s="10" r="I9">
         <v>0</v>
@@ -757,20 +757,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="R9"/>
-      <c s="13" r="S9">
-        <v>73</v>
+      <c s="12" r="S9">
+        <v>74</v>
       </c>
       <c s="5" t="str" r="T9"/>
       <c s="10" r="U9">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c s="5" t="str" r="V9"/>
-      <c s="11" r="W9">
-        <v>178</v>
+      <c s="13" r="W9">
+        <v>179</v>
       </c>
       <c s="5" t="str" r="X9"/>
-      <c s="11" r="Y9">
-        <v>178</v>
+      <c s="13" r="Y9">
+        <v>179</v>
       </c>
       <c s="5" t="str" r="Z9"/>
     </row>
@@ -784,14 +784,14 @@
       <c s="4" t="str" r="C10"/>
       <c s="5" t="str" r="D10"/>
       <c s="7" r="E10">
-        <v>339</v>
+        <v>295</v>
       </c>
       <c s="11" r="F10">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c s="5" t="str" r="G10"/>
-      <c s="9" r="H10">
-        <v>3</v>
+      <c s="8" r="H10">
+        <v>6</v>
       </c>
       <c s="10" r="I10">
         <v>0</v>
@@ -813,19 +813,19 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="R10"/>
-      <c s="13" r="S10">
-        <v>65</v>
+      <c s="12" r="S10">
+        <v>67</v>
       </c>
       <c s="5" t="str" r="T10"/>
       <c s="10" r="U10">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c s="5" t="str" r="V10"/>
-      <c s="12" r="W10">
+      <c s="11" r="W10">
         <v>183</v>
       </c>
       <c s="5" t="str" r="X10"/>
-      <c s="12" r="Y10">
+      <c s="11" r="Y10">
         <v>183</v>
       </c>
       <c s="5" t="str" r="Z10"/>
@@ -840,14 +840,14 @@
       <c s="4" t="str" r="C11"/>
       <c s="5" t="str" r="D11"/>
       <c s="7" r="E11">
-        <v>263</v>
+        <v>230</v>
       </c>
       <c s="11" r="F11">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c s="5" t="str" r="G11"/>
       <c s="9" r="H11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c s="10" r="I11">
         <v>0</v>
@@ -865,24 +865,24 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="P11"/>
-      <c s="9" r="Q11">
-        <v>12</v>
+      <c s="12" r="Q11">
+        <v>39</v>
       </c>
       <c s="5" t="str" r="R11"/>
-      <c s="13" r="S11">
-        <v>78</v>
+      <c s="12" r="S11">
+        <v>104</v>
       </c>
       <c s="5" t="str" r="T11"/>
       <c s="10" r="U11">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c s="5" t="str" r="V11"/>
-      <c s="8" r="W11">
-        <v>132</v>
+      <c s="13" r="W11">
+        <v>192</v>
       </c>
       <c s="5" t="str" r="X11"/>
-      <c s="8" r="Y11">
-        <v>170</v>
+      <c s="11" r="Y11">
+        <v>297</v>
       </c>
       <c s="5" t="str" r="Z11"/>
     </row>
@@ -896,7 +896,7 @@
       <c s="4" t="str" r="C12"/>
       <c s="5" t="str" r="D12"/>
       <c s="7" r="E12">
-        <v>329</v>
+        <v>293</v>
       </c>
       <c s="10" r="F12">
         <v>0</v>
@@ -905,8 +905,8 @@
       <c s="10" r="H12">
         <v>0</v>
       </c>
-      <c s="13" r="I12">
-        <v>37</v>
+      <c s="12" r="I12">
+        <v>35</v>
       </c>
       <c s="5" t="str" r="J12"/>
       <c s="9" r="K12">
@@ -914,7 +914,7 @@
       </c>
       <c s="5" t="str" r="L12"/>
       <c s="9" r="M12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c s="5" t="str" r="N12"/>
       <c s="9" r="O12">
@@ -925,20 +925,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="R12"/>
-      <c s="13" r="S12">
-        <v>70</v>
+      <c s="12" r="S12">
+        <v>74</v>
       </c>
       <c s="5" t="str" r="T12"/>
       <c s="10" r="U12">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c s="5" t="str" r="V12"/>
       <c s="11" r="W12">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c s="5" t="str" r="X12"/>
       <c s="11" r="Y12">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c s="5" t="str" r="Z12"/>
     </row>
@@ -952,14 +952,14 @@
       <c s="4" t="str" r="C13"/>
       <c s="5" t="str" r="D13"/>
       <c s="7" r="E13">
-        <v>401</v>
+        <v>349</v>
       </c>
       <c s="8" r="F13">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c s="5" t="str" r="G13"/>
       <c s="9" r="H13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c s="10" r="I13">
         <v>0</v>
@@ -977,24 +977,24 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="P13"/>
-      <c s="8" r="Q13">
-        <v>18</v>
+      <c s="9" r="Q13">
+        <v>11</v>
       </c>
       <c s="5" t="str" r="R13"/>
-      <c s="13" r="S13">
-        <v>60</v>
+      <c s="12" r="S13">
+        <v>56</v>
       </c>
       <c s="5" t="str" r="T13"/>
       <c s="10" r="U13">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c s="5" t="str" r="V13"/>
-      <c s="8" r="W13">
-        <v>175</v>
+      <c s="9" r="W13">
+        <v>138</v>
       </c>
       <c s="5" t="str" r="X13"/>
-      <c s="8" r="Y13">
-        <v>175</v>
+      <c s="9" r="Y13">
+        <v>138</v>
       </c>
       <c s="5" t="str" r="Z13"/>
     </row>
@@ -1103,12 +1103,12 @@
       <c s="4" t="str" r="E16"/>
       <c s="5" t="str" r="F16"/>
       <c s="19" r="G16">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c s="4" t="str" r="H16"/>
       <c s="5" t="str" r="I16"/>
       <c s="20" r="J16">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c s="5" t="str" r="K16"/>
       <c s="21" r="L16">
@@ -1136,19 +1136,19 @@
       </c>
       <c s="5" t="str" r="W16"/>
       <c s="20" r="X16">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c s="5" t="str" r="Y16"/>
       <c s="22" r="Z16">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c s="5" t="str" r="AA16"/>
       <c s="21" r="AB16">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c s="5" t="str" r="AC16"/>
       <c s="21" r="AD16">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" ht="18" customHeight="0">
@@ -1161,16 +1161,16 @@
       <c s="4" t="str" r="E17"/>
       <c s="5" t="str" r="F17"/>
       <c s="19" r="G17">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c s="4" t="str" r="H17"/>
       <c s="5" t="str" r="I17"/>
       <c s="20" r="J17">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c s="5" t="str" r="K17"/>
       <c s="21" r="L17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c s="5" t="str" r="M17"/>
       <c s="22" r="N17">
@@ -1193,20 +1193,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W17"/>
-      <c s="24" r="X17">
-        <v>60</v>
+      <c s="20" r="X17">
+        <v>59</v>
       </c>
       <c s="5" t="str" r="Y17"/>
       <c s="22" r="Z17">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c s="5" t="str" r="AA17"/>
       <c s="24" r="AB17">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c s="5" t="str" r="AC17"/>
       <c s="21" r="AD17">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" ht="18" customHeight="0">
@@ -1219,16 +1219,16 @@
       <c s="4" t="str" r="E18"/>
       <c s="5" t="str" r="F18"/>
       <c s="19" r="G18">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c s="4" t="str" r="H18"/>
       <c s="5" t="str" r="I18"/>
       <c s="20" r="J18">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c s="5" t="str" r="K18"/>
       <c s="21" r="L18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M18"/>
       <c s="22" r="N18">
@@ -1251,26 +1251,26 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W18"/>
-      <c s="25" r="X18">
-        <v>102</v>
+      <c s="24" r="X18">
+        <v>67</v>
       </c>
       <c s="5" t="str" r="Y18"/>
       <c s="22" r="Z18">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c s="5" t="str" r="AA18"/>
-      <c s="24" r="AB18">
-        <v>196</v>
+      <c s="21" r="AB18">
+        <v>120</v>
       </c>
       <c s="5" t="str" r="AC18"/>
-      <c s="20" r="AD18">
-        <v>97</v>
+      <c s="21" r="AD18">
+        <v>60</v>
       </c>
     </row>
     <row r="19" ht="18" customHeight="0">
-      <c s="26" t="str" r="A19"/>
-      <c s="27" t="str" r="B19"/>
-      <c s="27" t="str" r="C19"/>
+      <c s="25" t="str" r="A19"/>
+      <c s="26" t="str" r="B19"/>
+      <c s="26" t="str" r="C19"/>
       <c s="18" t="inlineStr" r="D19">
         <is>
           <t xml:space="preserve">Daypart 5</t>
@@ -1279,12 +1279,12 @@
       <c s="4" t="str" r="E19"/>
       <c s="5" t="str" r="F19"/>
       <c s="19" r="G19">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c s="4" t="str" r="H19"/>
       <c s="5" t="str" r="I19"/>
       <c s="20" r="J19">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c s="5" t="str" r="K19"/>
       <c s="21" r="L19">
@@ -1311,20 +1311,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W19"/>
-      <c s="25" r="X19">
-        <v>91</v>
+      <c s="24" r="X19">
+        <v>65</v>
       </c>
       <c s="5" t="str" r="Y19"/>
       <c s="22" r="Z19">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c s="5" t="str" r="AA19"/>
       <c s="21" r="AB19">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c s="5" t="str" r="AC19"/>
       <c s="21" r="AD19">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" ht="18" customHeight="0">
@@ -1347,8 +1347,8 @@
       </c>
       <c s="4" t="str" r="H20"/>
       <c s="5" t="str" r="I20"/>
-      <c s="21" r="J20">
-        <v>19</v>
+      <c s="20" r="J20">
+        <v>24</v>
       </c>
       <c s="5" t="str" r="K20"/>
       <c s="20" r="L20">
@@ -1375,20 +1375,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W20"/>
-      <c s="28" r="X20">
-        <v>48</v>
+      <c s="27" r="X20">
+        <v>77</v>
       </c>
       <c s="5" t="str" r="Y20"/>
       <c s="22" r="Z20">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c s="5" t="str" r="AA20"/>
       <c s="21" r="AB20">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c s="5" t="str" r="AC20"/>
       <c s="21" r="AD20">
-        <v>78</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" ht="18" customHeight="0">
@@ -1401,12 +1401,12 @@
       <c s="4" t="str" r="E21"/>
       <c s="5" t="str" r="F21"/>
       <c s="19" r="G21">
-        <v>221</v>
+        <v>173</v>
       </c>
       <c s="4" t="str" r="H21"/>
       <c s="5" t="str" r="I21"/>
-      <c s="25" r="J21">
-        <v>31</v>
+      <c s="24" r="J21">
+        <v>26</v>
       </c>
       <c s="5" t="str" r="K21"/>
       <c s="21" r="L21">
@@ -1434,19 +1434,19 @@
       </c>
       <c s="5" t="str" r="W21"/>
       <c s="28" r="X21">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c s="5" t="str" r="Y21"/>
       <c s="22" r="Z21">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c s="5" t="str" r="AA21"/>
-      <c s="20" r="AB21">
-        <v>156</v>
+      <c s="21" r="AB21">
+        <v>112</v>
       </c>
       <c s="5" t="str" r="AC21"/>
-      <c s="20" r="AD21">
-        <v>156</v>
+      <c s="21" r="AD21">
+        <v>112</v>
       </c>
     </row>
     <row r="22" ht="18" customHeight="0">
@@ -1459,16 +1459,16 @@
       <c s="4" t="str" r="E22"/>
       <c s="5" t="str" r="F22"/>
       <c s="19" r="G22">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c s="4" t="str" r="H22"/>
       <c s="5" t="str" r="I22"/>
-      <c s="25" r="J22">
+      <c s="28" r="J22">
         <v>34</v>
       </c>
       <c s="5" t="str" r="K22"/>
       <c s="21" r="L22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c s="5" t="str" r="M22"/>
       <c s="22" r="N22">
@@ -1491,20 +1491,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W22"/>
-      <c s="28" r="X22">
-        <v>53</v>
+      <c s="27" r="X22">
+        <v>48</v>
       </c>
       <c s="5" t="str" r="Y22"/>
       <c s="22" r="Z22">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c s="5" t="str" r="AA22"/>
-      <c s="20" r="AB22">
-        <v>156</v>
+      <c s="21" r="AB22">
+        <v>136</v>
       </c>
       <c s="5" t="str" r="AC22"/>
-      <c s="20" r="AD22">
-        <v>156</v>
+      <c s="21" r="AD22">
+        <v>136</v>
       </c>
     </row>
     <row r="23" ht="18" customHeight="0">
@@ -1517,12 +1517,12 @@
       <c s="4" t="str" r="E23"/>
       <c s="5" t="str" r="F23"/>
       <c s="19" r="G23">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c s="4" t="str" r="H23"/>
       <c s="5" t="str" r="I23"/>
       <c s="28" r="J23">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c s="5" t="str" r="K23"/>
       <c s="21" r="L23">
@@ -1549,26 +1549,26 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W23"/>
-      <c s="28" r="X23">
-        <v>69</v>
+      <c s="27" r="X23">
+        <v>74</v>
       </c>
       <c s="5" t="str" r="Y23"/>
       <c s="22" r="Z23">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c s="5" t="str" r="AA23"/>
-      <c s="24" r="AB23">
-        <v>169</v>
+      <c s="20" r="AB23">
+        <v>150</v>
       </c>
       <c s="5" t="str" r="AC23"/>
-      <c s="24" r="AD23">
-        <v>169</v>
+      <c s="20" r="AD23">
+        <v>150</v>
       </c>
     </row>
     <row r="24" ht="18" customHeight="0">
-      <c s="26" t="str" r="A24"/>
-      <c s="27" t="str" r="B24"/>
-      <c s="27" t="str" r="C24"/>
+      <c s="25" t="str" r="A24"/>
+      <c s="26" t="str" r="B24"/>
+      <c s="26" t="str" r="C24"/>
       <c s="18" t="inlineStr" r="D24">
         <is>
           <t xml:space="preserve">Daypart 5</t>
@@ -1577,16 +1577,16 @@
       <c s="4" t="str" r="E24"/>
       <c s="5" t="str" r="F24"/>
       <c s="19" r="G24">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c s="4" t="str" r="H24"/>
       <c s="5" t="str" r="I24"/>
-      <c s="28" r="J24">
-        <v>35</v>
+      <c s="24" r="J24">
+        <v>26</v>
       </c>
       <c s="5" t="str" r="K24"/>
-      <c s="20" r="L24">
-        <v>6</v>
+      <c s="21" r="L24">
+        <v>1</v>
       </c>
       <c s="5" t="str" r="M24"/>
       <c s="22" r="N24">
@@ -1609,20 +1609,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W24"/>
-      <c s="28" r="X24">
-        <v>116</v>
+      <c s="27" r="X24">
+        <v>62</v>
       </c>
       <c s="5" t="str" r="Y24"/>
       <c s="22" r="Z24">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c s="5" t="str" r="AA24"/>
-      <c s="25" r="AB24">
-        <v>180</v>
+      <c s="21" r="AB24">
+        <v>99</v>
       </c>
       <c s="5" t="str" r="AC24"/>
-      <c s="25" r="AD24">
-        <v>180</v>
+      <c s="21" r="AD24">
+        <v>99</v>
       </c>
     </row>
     <row r="25" ht="18" customHeight="0">
@@ -1641,16 +1641,16 @@
       <c s="4" t="str" r="E25"/>
       <c s="5" t="str" r="F25"/>
       <c s="19" r="G25">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c s="4" t="str" r="H25"/>
       <c s="5" t="str" r="I25"/>
       <c s="28" r="J25">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c s="5" t="str" r="K25"/>
-      <c s="24" r="L25">
-        <v>7</v>
+      <c s="20" r="L25">
+        <v>5</v>
       </c>
       <c s="5" t="str" r="M25"/>
       <c s="22" r="N25">
@@ -1673,20 +1673,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W25"/>
-      <c s="28" r="X25">
-        <v>64</v>
+      <c s="27" r="X25">
+        <v>59</v>
       </c>
       <c s="5" t="str" r="Y25"/>
       <c s="22" r="Z25">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c s="5" t="str" r="AA25"/>
-      <c s="24" r="AB25">
-        <v>171</v>
+      <c s="21" r="AB25">
+        <v>135</v>
       </c>
       <c s="5" t="str" r="AC25"/>
-      <c s="24" r="AD25">
-        <v>171</v>
+      <c s="21" r="AD25">
+        <v>135</v>
       </c>
     </row>
     <row r="26" ht="18" customHeight="0">
@@ -1699,16 +1699,16 @@
       <c s="4" t="str" r="E26"/>
       <c s="5" t="str" r="F26"/>
       <c s="19" r="G26">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c s="4" t="str" r="H26"/>
       <c s="5" t="str" r="I26"/>
-      <c s="28" r="J26">
-        <v>51</v>
+      <c s="27" r="J26">
+        <v>44</v>
       </c>
       <c s="5" t="str" r="K26"/>
-      <c s="25" r="L26">
-        <v>11</v>
+      <c s="27" r="L26">
+        <v>12</v>
       </c>
       <c s="5" t="str" r="M26"/>
       <c s="22" r="N26">
@@ -1731,20 +1731,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W26"/>
-      <c s="28" r="X26">
-        <v>63</v>
+      <c s="27" r="X26">
+        <v>66</v>
       </c>
       <c s="5" t="str" r="Y26"/>
       <c s="22" r="Z26">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c s="5" t="str" r="AA26"/>
-      <c s="24" r="AB26">
-        <v>173</v>
+      <c s="28" r="AB26">
+        <v>180</v>
       </c>
       <c s="5" t="str" r="AC26"/>
-      <c s="24" r="AD26">
-        <v>173</v>
+      <c s="28" r="AD26">
+        <v>180</v>
       </c>
     </row>
     <row r="27" ht="18" customHeight="0">
@@ -1757,16 +1757,16 @@
       <c s="4" t="str" r="E27"/>
       <c s="5" t="str" r="F27"/>
       <c s="19" r="G27">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c s="4" t="str" r="H27"/>
       <c s="5" t="str" r="I27"/>
-      <c s="28" r="J27">
-        <v>50</v>
+      <c s="27" r="J27">
+        <v>77</v>
       </c>
       <c s="5" t="str" r="K27"/>
-      <c s="25" r="L27">
-        <v>10</v>
+      <c s="27" r="L27">
+        <v>21</v>
       </c>
       <c s="5" t="str" r="M27"/>
       <c s="22" r="N27">
@@ -1789,26 +1789,26 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W27"/>
-      <c s="28" r="X27">
-        <v>99</v>
+      <c s="27" r="X27">
+        <v>106</v>
       </c>
       <c s="5" t="str" r="Y27"/>
       <c s="22" r="Z27">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c s="5" t="str" r="AA27"/>
-      <c s="28" r="AB27">
-        <v>199</v>
+      <c s="27" r="AB27">
+        <v>252</v>
       </c>
       <c s="5" t="str" r="AC27"/>
-      <c s="28" r="AD27">
-        <v>199</v>
+      <c s="27" r="AD27">
+        <v>252</v>
       </c>
     </row>
     <row r="28" ht="18" customHeight="0">
-      <c s="26" t="str" r="A28"/>
-      <c s="27" t="str" r="B28"/>
-      <c s="27" t="str" r="C28"/>
+      <c s="25" t="str" r="A28"/>
+      <c s="26" t="str" r="B28"/>
+      <c s="26" t="str" r="C28"/>
       <c s="18" t="inlineStr" r="D28">
         <is>
           <t xml:space="preserve">Daypart 5</t>
@@ -1817,16 +1817,16 @@
       <c s="4" t="str" r="E28"/>
       <c s="5" t="str" r="F28"/>
       <c s="19" r="G28">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c s="4" t="str" r="H28"/>
       <c s="5" t="str" r="I28"/>
-      <c s="28" r="J28">
-        <v>45</v>
+      <c s="27" r="J28">
+        <v>71</v>
       </c>
       <c s="5" t="str" r="K28"/>
       <c s="20" r="L28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c s="5" t="str" r="M28"/>
       <c s="22" r="N28">
@@ -1849,20 +1849,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W28"/>
-      <c s="28" r="X28">
-        <v>135</v>
+      <c s="27" r="X28">
+        <v>122</v>
       </c>
       <c s="5" t="str" r="Y28"/>
       <c s="22" r="Z28">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c s="5" t="str" r="AA28"/>
-      <c s="28" r="AB28">
-        <v>207</v>
+      <c s="27" r="AB28">
+        <v>199</v>
       </c>
       <c s="5" t="str" r="AC28"/>
-      <c s="28" r="AD28">
-        <v>207</v>
+      <c s="27" r="AD28">
+        <v>199</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="0">
@@ -1881,16 +1881,16 @@
       <c s="4" t="str" r="E29"/>
       <c s="5" t="str" r="F29"/>
       <c s="19" r="G29">
-        <v>152</v>
+        <v>115</v>
       </c>
       <c s="4" t="str" r="H29"/>
       <c s="5" t="str" r="I29"/>
       <c s="20" r="J29">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c s="5" t="str" r="K29"/>
       <c s="21" r="L29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M29"/>
       <c s="22" r="N29">
@@ -1913,20 +1913,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W29"/>
-      <c s="28" r="X29">
+      <c s="27" r="X29">
         <v>58</v>
       </c>
       <c s="5" t="str" r="Y29"/>
       <c s="22" r="Z29">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c s="5" t="str" r="AA29"/>
-      <c s="24" r="AB29">
-        <v>170</v>
+      <c s="21" r="AB29">
+        <v>139</v>
       </c>
       <c s="5" t="str" r="AC29"/>
-      <c s="24" r="AD29">
-        <v>170</v>
+      <c s="21" r="AD29">
+        <v>139</v>
       </c>
     </row>
     <row r="30" ht="18" customHeight="0">
@@ -1939,16 +1939,16 @@
       <c s="4" t="str" r="E30"/>
       <c s="5" t="str" r="F30"/>
       <c s="19" r="G30">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c s="4" t="str" r="H30"/>
       <c s="5" t="str" r="I30"/>
-      <c s="25" r="J30">
-        <v>32</v>
+      <c s="27" r="J30">
+        <v>39</v>
       </c>
       <c s="5" t="str" r="K30"/>
-      <c s="21" r="L30">
-        <v>3</v>
+      <c s="24" r="L30">
+        <v>8</v>
       </c>
       <c s="5" t="str" r="M30"/>
       <c s="22" r="N30">
@@ -1971,20 +1971,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W30"/>
-      <c s="28" r="X30">
-        <v>65</v>
+      <c s="27" r="X30">
+        <v>69</v>
       </c>
       <c s="5" t="str" r="Y30"/>
       <c s="22" r="Z30">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c s="5" t="str" r="AA30"/>
-      <c s="28" r="AB30">
-        <v>210</v>
+      <c s="27" r="AB30">
+        <v>234</v>
       </c>
       <c s="5" t="str" r="AC30"/>
-      <c s="28" r="AD30">
-        <v>210</v>
+      <c s="27" r="AD30">
+        <v>234</v>
       </c>
     </row>
     <row r="31" ht="18" customHeight="0">
@@ -1997,16 +1997,16 @@
       <c s="4" t="str" r="E31"/>
       <c s="5" t="str" r="F31"/>
       <c s="19" r="G31">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c s="4" t="str" r="H31"/>
       <c s="5" t="str" r="I31"/>
-      <c s="28" r="J31">
-        <v>41</v>
+      <c s="27" r="J31">
+        <v>39</v>
       </c>
       <c s="5" t="str" r="K31"/>
-      <c s="24" r="L31">
-        <v>9</v>
+      <c s="28" r="L31">
+        <v>10</v>
       </c>
       <c s="5" t="str" r="M31"/>
       <c s="22" r="N31">
@@ -2029,26 +2029,26 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W31"/>
-      <c s="28" r="X31">
-        <v>78</v>
+      <c s="27" r="X31">
+        <v>84</v>
       </c>
       <c s="5" t="str" r="Y31"/>
       <c s="22" r="Z31">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c s="5" t="str" r="AA31"/>
-      <c s="21" r="AB31">
-        <v>138</v>
+      <c s="20" r="AB31">
+        <v>150</v>
       </c>
       <c s="5" t="str" r="AC31"/>
-      <c s="21" r="AD31">
-        <v>138</v>
+      <c s="20" r="AD31">
+        <v>150</v>
       </c>
     </row>
     <row r="32" ht="18" customHeight="0">
-      <c s="26" t="str" r="A32"/>
-      <c s="27" t="str" r="B32"/>
-      <c s="27" t="str" r="C32"/>
+      <c s="25" t="str" r="A32"/>
+      <c s="26" t="str" r="B32"/>
+      <c s="26" t="str" r="C32"/>
       <c s="18" t="inlineStr" r="D32">
         <is>
           <t xml:space="preserve">Daypart 5</t>
@@ -2057,16 +2057,16 @@
       <c s="4" t="str" r="E32"/>
       <c s="5" t="str" r="F32"/>
       <c s="19" r="G32">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c s="4" t="str" r="H32"/>
       <c s="5" t="str" r="I32"/>
-      <c s="25" r="J32">
-        <v>33</v>
+      <c s="27" r="J32">
+        <v>44</v>
       </c>
       <c s="5" t="str" r="K32"/>
-      <c s="21" r="L32">
-        <v>4</v>
+      <c s="20" r="L32">
+        <v>6</v>
       </c>
       <c s="5" t="str" r="M32"/>
       <c s="22" r="N32">
@@ -2089,20 +2089,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W32"/>
-      <c s="28" r="X32">
-        <v>105</v>
+      <c s="27" r="X32">
+        <v>75</v>
       </c>
       <c s="5" t="str" r="Y32"/>
       <c s="22" r="Z32">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c s="5" t="str" r="AA32"/>
-      <c s="20" r="AB32">
-        <v>162</v>
+      <c s="21" r="AB32">
+        <v>132</v>
       </c>
       <c s="5" t="str" r="AC32"/>
-      <c s="20" r="AD32">
-        <v>162</v>
+      <c s="21" r="AD32">
+        <v>132</v>
       </c>
     </row>
     <row r="33" ht="18" customHeight="0">
@@ -2121,12 +2121,12 @@
       <c s="4" t="str" r="E33"/>
       <c s="5" t="str" r="F33"/>
       <c s="19" r="G33">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c s="4" t="str" r="H33"/>
       <c s="5" t="str" r="I33"/>
       <c s="20" r="J33">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c s="5" t="str" r="K33"/>
       <c s="21" r="L33">
@@ -2150,23 +2150,23 @@
       </c>
       <c s="5" t="str" r="U33"/>
       <c s="21" r="V33">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c s="5" t="str" r="W33"/>
-      <c s="28" r="X33">
-        <v>61</v>
+      <c s="27" r="X33">
+        <v>85</v>
       </c>
       <c s="5" t="str" r="Y33"/>
       <c s="22" r="Z33">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c s="5" t="str" r="AA33"/>
-      <c s="21" r="AB33">
-        <v>111</v>
+      <c s="20" r="AB33">
+        <v>121</v>
       </c>
       <c s="5" t="str" r="AC33"/>
       <c s="20" r="AD33">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" ht="18" customHeight="0">
@@ -2179,16 +2179,16 @@
       <c s="4" t="str" r="E34"/>
       <c s="5" t="str" r="F34"/>
       <c s="19" r="G34">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c s="4" t="str" r="H34"/>
       <c s="5" t="str" r="I34"/>
-      <c s="24" r="J34">
-        <v>44</v>
+      <c s="27" r="J34">
+        <v>68</v>
       </c>
       <c s="5" t="str" r="K34"/>
-      <c s="21" r="L34">
-        <v>4</v>
+      <c s="20" r="L34">
+        <v>5</v>
       </c>
       <c s="5" t="str" r="M34"/>
       <c s="22" r="N34">
@@ -2207,24 +2207,24 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="U34"/>
-      <c s="21" r="V34">
-        <v>14</v>
+      <c s="27" r="V34">
+        <v>85</v>
       </c>
       <c s="5" t="str" r="W34"/>
-      <c s="28" r="X34">
-        <v>80</v>
+      <c s="27" r="X34">
+        <v>127</v>
       </c>
       <c s="5" t="str" r="Y34"/>
       <c s="22" r="Z34">
-        <v>42</v>
+        <v>196</v>
       </c>
       <c s="5" t="str" r="AA34"/>
-      <c s="20" r="AB34">
-        <v>136</v>
+      <c s="28" r="AB34">
+        <v>275</v>
       </c>
       <c s="5" t="str" r="AC34"/>
-      <c s="20" r="AD34">
-        <v>178</v>
+      <c s="27" r="AD34">
+        <v>471</v>
       </c>
     </row>
     <row r="35" ht="18" customHeight="0">
@@ -2237,16 +2237,16 @@
       <c s="4" t="str" r="E35"/>
       <c s="5" t="str" r="F35"/>
       <c s="19" r="G35">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c s="4" t="str" r="H35"/>
       <c s="5" t="str" r="I35"/>
-      <c s="24" r="J35">
-        <v>46</v>
+      <c s="28" r="J35">
+        <v>54</v>
       </c>
       <c s="5" t="str" r="K35"/>
       <c s="21" r="L35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c s="5" t="str" r="M35"/>
       <c s="22" r="N35">
@@ -2266,29 +2266,29 @@
       </c>
       <c s="5" t="str" r="U35"/>
       <c s="21" r="V35">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c s="5" t="str" r="W35"/>
-      <c s="28" r="X35">
-        <v>98</v>
+      <c s="27" r="X35">
+        <v>100</v>
       </c>
       <c s="5" t="str" r="Y35"/>
       <c s="22" r="Z35">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c s="5" t="str" r="AA35"/>
       <c s="20" r="AB35">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c s="5" t="str" r="AC35"/>
-      <c s="20" r="AD35">
-        <v>179</v>
+      <c s="24" r="AD35">
+        <v>206</v>
       </c>
     </row>
     <row r="36" ht="18" customHeight="0">
-      <c s="26" t="str" r="A36"/>
-      <c s="27" t="str" r="B36"/>
-      <c s="27" t="str" r="C36"/>
+      <c s="25" t="str" r="A36"/>
+      <c s="26" t="str" r="B36"/>
+      <c s="26" t="str" r="C36"/>
       <c s="18" t="inlineStr" r="D36">
         <is>
           <t xml:space="preserve">Daypart 5</t>
@@ -2297,16 +2297,16 @@
       <c s="4" t="str" r="E36"/>
       <c s="5" t="str" r="F36"/>
       <c s="19" r="G36">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c s="4" t="str" r="H36"/>
       <c s="5" t="str" r="I36"/>
       <c s="28" r="J36">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c s="5" t="str" r="K36"/>
-      <c s="21" r="L36">
-        <v>4</v>
+      <c s="20" r="L36">
+        <v>5</v>
       </c>
       <c s="5" t="str" r="M36"/>
       <c s="22" r="N36">
@@ -2326,23 +2326,23 @@
       </c>
       <c s="5" t="str" r="U36"/>
       <c s="21" r="V36">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c s="5" t="str" r="W36"/>
-      <c s="28" r="X36">
-        <v>138</v>
+      <c s="27" r="X36">
+        <v>78</v>
       </c>
       <c s="5" t="str" r="Y36"/>
       <c s="22" r="Z36">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c s="5" t="str" r="AA36"/>
-      <c s="24" r="AB36">
-        <v>211</v>
+      <c s="20" r="AB36">
+        <v>127</v>
       </c>
       <c s="5" t="str" r="AC36"/>
-      <c s="24" r="AD36">
-        <v>224</v>
+      <c s="20" r="AD36">
+        <v>160</v>
       </c>
     </row>
     <row r="37" ht="18" customHeight="0">
@@ -2361,7 +2361,7 @@
       <c s="4" t="str" r="E37"/>
       <c s="5" t="str" r="F37"/>
       <c s="19" r="G37">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c s="4" t="str" r="H37"/>
       <c s="5" t="str" r="I37"/>
@@ -2374,39 +2374,39 @@
       </c>
       <c s="5" t="str" r="M37"/>
       <c s="28" r="N37">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c s="5" t="str" r="O37"/>
       <c s="21" r="P37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c s="5" t="str" r="Q37"/>
       <c s="21" r="R37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c s="5" t="str" r="S37"/>
       <c s="21" r="T37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c s="5" t="str" r="U37"/>
       <c s="22" r="V37">
         <v>0</v>
       </c>
       <c s="5" t="str" r="W37"/>
-      <c s="28" r="X37">
-        <v>58</v>
+      <c s="27" r="X37">
+        <v>74</v>
       </c>
       <c s="5" t="str" r="Y37"/>
       <c s="22" r="Z37">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c s="5" t="str" r="AA37"/>
-      <c s="20" r="AB37">
-        <v>162</v>
+      <c s="27" r="AB37">
+        <v>203</v>
       </c>
       <c s="5" t="str" r="AC37"/>
-      <c s="20" r="AD37">
-        <v>162</v>
+      <c s="27" r="AD37">
+        <v>203</v>
       </c>
     </row>
     <row r="38" ht="18" customHeight="0">
@@ -2419,7 +2419,7 @@
       <c s="4" t="str" r="E38"/>
       <c s="5" t="str" r="F38"/>
       <c s="19" r="G38">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c s="4" t="str" r="H38"/>
       <c s="5" t="str" r="I38"/>
@@ -2432,11 +2432,11 @@
       </c>
       <c s="5" t="str" r="M38"/>
       <c s="28" r="N38">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c s="5" t="str" r="O38"/>
       <c s="21" r="P38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c s="5" t="str" r="Q38"/>
       <c s="21" r="R38">
@@ -2451,20 +2451,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W38"/>
-      <c s="28" r="X38">
-        <v>77</v>
+      <c s="27" r="X38">
+        <v>74</v>
       </c>
       <c s="5" t="str" r="Y38"/>
       <c s="22" r="Z38">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c s="5" t="str" r="AA38"/>
-      <c s="28" r="AB38">
-        <v>216</v>
+      <c s="27" r="AB38">
+        <v>203</v>
       </c>
       <c s="5" t="str" r="AC38"/>
-      <c s="28" r="AD38">
-        <v>216</v>
+      <c s="27" r="AD38">
+        <v>203</v>
       </c>
     </row>
     <row r="39" ht="18" customHeight="0">
@@ -2477,7 +2477,7 @@
       <c s="4" t="str" r="E39"/>
       <c s="5" t="str" r="F39"/>
       <c s="19" r="G39">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c s="4" t="str" r="H39"/>
       <c s="5" t="str" r="I39"/>
@@ -2489,12 +2489,12 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="M39"/>
-      <c s="28" r="N39">
-        <v>45</v>
+      <c s="27" r="N39">
+        <v>44</v>
       </c>
       <c s="5" t="str" r="O39"/>
       <c s="21" r="P39">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c s="5" t="str" r="Q39"/>
       <c s="21" r="R39">
@@ -2509,26 +2509,26 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W39"/>
-      <c s="28" r="X39">
-        <v>89</v>
+      <c s="27" r="X39">
+        <v>73</v>
       </c>
       <c s="5" t="str" r="Y39"/>
       <c s="22" r="Z39">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c s="5" t="str" r="AA39"/>
-      <c s="24" r="AB39">
-        <v>172</v>
+      <c s="21" r="AB39">
+        <v>144</v>
       </c>
       <c s="5" t="str" r="AC39"/>
-      <c s="24" r="AD39">
-        <v>172</v>
+      <c s="21" r="AD39">
+        <v>144</v>
       </c>
     </row>
     <row r="40" ht="18" customHeight="0">
-      <c s="26" t="str" r="A40"/>
-      <c s="27" t="str" r="B40"/>
-      <c s="27" t="str" r="C40"/>
+      <c s="25" t="str" r="A40"/>
+      <c s="26" t="str" r="B40"/>
+      <c s="26" t="str" r="C40"/>
       <c s="18" t="inlineStr" r="D40">
         <is>
           <t xml:space="preserve">Daypart 5</t>
@@ -2537,7 +2537,7 @@
       <c s="4" t="str" r="E40"/>
       <c s="5" t="str" r="F40"/>
       <c s="19" r="G40">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c s="4" t="str" r="H40"/>
       <c s="5" t="str" r="I40"/>
@@ -2549,12 +2549,12 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="M40"/>
-      <c s="20" r="N40">
-        <v>24</v>
+      <c s="28" r="N40">
+        <v>31</v>
       </c>
       <c s="5" t="str" r="O40"/>
       <c s="21" r="P40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c s="5" t="str" r="Q40"/>
       <c s="21" r="R40">
@@ -2569,20 +2569,20 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="W40"/>
-      <c s="28" r="X40">
-        <v>51</v>
+      <c s="27" r="X40">
+        <v>79</v>
       </c>
       <c s="5" t="str" r="Y40"/>
       <c s="22" r="Z40">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c s="5" t="str" r="AA40"/>
       <c s="21" r="AB40">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c s="5" t="str" r="AC40"/>
       <c s="21" r="AD40">
-        <v>81</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" ht="18" customHeight="0">
@@ -2601,16 +2601,16 @@
       <c s="4" t="str" r="E41"/>
       <c s="5" t="str" r="F41"/>
       <c s="19" r="G41">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c s="4" t="str" r="H41"/>
       <c s="5" t="str" r="I41"/>
-      <c s="20" r="J41">
-        <v>35</v>
+      <c s="21" r="J41">
+        <v>28</v>
       </c>
       <c s="5" t="str" r="K41"/>
       <c s="21" r="L41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c s="5" t="str" r="M41"/>
       <c s="22" r="N41">
@@ -2629,24 +2629,24 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="U41"/>
-      <c s="20" r="V41">
-        <v>17</v>
+      <c s="21" r="V41">
+        <v>13</v>
       </c>
       <c s="5" t="str" r="W41"/>
-      <c s="28" r="X41">
-        <v>54</v>
+      <c s="27" r="X41">
+        <v>46</v>
       </c>
       <c s="5" t="str" r="Y41"/>
       <c s="22" r="Z41">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c s="5" t="str" r="AA41"/>
-      <c s="20" r="AB41">
-        <v>168</v>
+      <c s="21" r="AB41">
+        <v>122</v>
       </c>
       <c s="5" t="str" r="AC41"/>
-      <c s="20" r="AD41">
-        <v>168</v>
+      <c s="21" r="AD41">
+        <v>122</v>
       </c>
     </row>
     <row r="42" ht="18" customHeight="0">
@@ -2659,16 +2659,16 @@
       <c s="4" t="str" r="E42"/>
       <c s="5" t="str" r="F42"/>
       <c s="19" r="G42">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c s="4" t="str" r="H42"/>
       <c s="5" t="str" r="I42"/>
       <c s="20" r="J42">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c s="5" t="str" r="K42"/>
       <c s="21" r="L42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c s="5" t="str" r="M42"/>
       <c s="22" r="N42">
@@ -2687,24 +2687,24 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="U42"/>
-      <c s="20" r="V42">
-        <v>19</v>
+      <c s="21" r="V42">
+        <v>14</v>
       </c>
       <c s="5" t="str" r="W42"/>
-      <c s="28" r="X42">
-        <v>56</v>
+      <c s="27" r="X42">
+        <v>57</v>
       </c>
       <c s="5" t="str" r="Y42"/>
       <c s="22" r="Z42">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c s="5" t="str" r="AA42"/>
       <c s="20" r="AB42">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c s="5" t="str" r="AC42"/>
       <c s="20" r="AD42">
-        <v>175</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" ht="18" customHeight="0">
@@ -2717,16 +2717,16 @@
       <c s="4" t="str" r="E43"/>
       <c s="5" t="str" r="F43"/>
       <c s="19" r="G43">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c s="4" t="str" r="H43"/>
       <c s="5" t="str" r="I43"/>
-      <c s="24" r="J43">
-        <v>44</v>
+      <c s="20" r="J43">
+        <v>38</v>
       </c>
       <c s="5" t="str" r="K43"/>
-      <c s="20" r="L43">
-        <v>6</v>
+      <c s="21" r="L43">
+        <v>3</v>
       </c>
       <c s="5" t="str" r="M43"/>
       <c s="22" r="N43">
@@ -2745,30 +2745,30 @@
         <v>0</v>
       </c>
       <c s="5" t="str" r="U43"/>
-      <c s="20" r="V43">
-        <v>18</v>
+      <c s="21" r="V43">
+        <v>3</v>
       </c>
       <c s="5" t="str" r="W43"/>
-      <c s="28" r="X43">
-        <v>84</v>
+      <c s="27" r="X43">
+        <v>73</v>
       </c>
       <c s="5" t="str" r="Y43"/>
       <c s="22" r="Z43">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c s="5" t="str" r="AA43"/>
-      <c s="24" r="AB43">
-        <v>207</v>
+      <c s="21" r="AB43">
+        <v>142</v>
       </c>
       <c s="5" t="str" r="AC43"/>
-      <c s="24" r="AD43">
-        <v>207</v>
+      <c s="21" r="AD43">
+        <v>142</v>
       </c>
     </row>
     <row r="44" ht="18" customHeight="0">
-      <c s="26" t="str" r="A44"/>
-      <c s="27" t="str" r="B44"/>
-      <c s="27" t="str" r="C44"/>
+      <c s="25" t="str" r="A44"/>
+      <c s="26" t="str" r="B44"/>
+      <c s="26" t="str" r="C44"/>
       <c s="18" t="inlineStr" r="D44">
         <is>
           <t xml:space="preserve">Daypart 5</t>
@@ -2777,12 +2777,12 @@
       <c s="4" t="str" r="E44"/>
       <c s="5" t="str" r="F44"/>
       <c s="19" r="G44">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c s="4" t="str" r="H44"/>
       <c s="5" t="str" r="I44"/>
-      <c s="24" r="J44">
-        <v>41</v>
+      <c s="21" r="J44">
+        <v>27</v>
       </c>
       <c s="5" t="str" r="K44"/>
       <c s="21" r="L44">
@@ -2806,23 +2806,23 @@
       </c>
       <c s="5" t="str" r="U44"/>
       <c s="21" r="V44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c s="5" t="str" r="W44"/>
-      <c s="28" r="X44">
-        <v>86</v>
+      <c s="27" r="X44">
+        <v>71</v>
       </c>
       <c s="5" t="str" r="Y44"/>
       <c s="22" r="Z44">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c s="5" t="str" r="AA44"/>
       <c s="21" r="AB44">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c s="5" t="str" r="AC44"/>
       <c s="21" r="AD44">
-        <v>136</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" ht="0.05" customHeight="1"/>
@@ -3291,7 +3291,7 @@
   <pageMargins left="0.2" right="0.2" top="0.5" bottom="0.95" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;L&amp;"Segoe UI,Italic"&amp;9 Print Date &amp;&amp; Time: 2/8/2026 12:41:16 PM 
+    <oddFooter>&amp;L&amp;"Segoe UI,Italic"&amp;9 Print Date &amp;&amp; Time: 2/9/2026 12:49:47 PM 
 &amp;"-,Italic"Page Number:  &amp;P </oddFooter>
   </headerFooter>
   <drawing r:id="rId7"/>

</xml_diff>